<commit_message>
Update input for paper (c2c).xlsx
</commit_message>
<xml_diff>
--- a/migforecasting/clustering/for paper/input for paper (c2c).xlsx
+++ b/migforecasting/clustering/for paper/input for paper (c2c).xlsx
@@ -402,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P46"/>
+  <dimension ref="A1:P91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V17" sqref="V17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -721,1252 +721,1252 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <v>4183.9999999999918</v>
+        <v>17499</v>
       </c>
       <c r="B7" s="2">
-        <v>788.99999999999841</v>
+        <v>2815</v>
       </c>
       <c r="C7" s="2">
-        <v>19068.8688</v>
+        <v>20675.747319999999</v>
       </c>
       <c r="D7" s="2">
-        <v>1820.9999999999964</v>
+        <v>4044.4999999999973</v>
       </c>
       <c r="E7" s="2">
-        <v>79.999999999999787</v>
+        <v>387.99999999999983</v>
       </c>
       <c r="F7" s="2">
-        <v>57968.611199999868</v>
+        <v>509272.59583999997</v>
       </c>
       <c r="G7" s="2">
-        <v>35.799999999999997</v>
+        <v>29.82</v>
       </c>
       <c r="H7" s="2">
-        <v>12.999999999999892</v>
+        <v>53.999999999999659</v>
       </c>
       <c r="I7" s="2">
-        <v>1.9999999999999847</v>
+        <v>31.999999999999865</v>
       </c>
       <c r="J7" s="2">
-        <v>81.399999999999764</v>
+        <v>1231.9999999999993</v>
       </c>
       <c r="K7" s="2">
-        <v>32010.999999999935</v>
+        <v>47001.999999999993</v>
       </c>
       <c r="L7" s="2">
-        <v>1244.4599999999969</v>
+        <v>8969.9999999999982</v>
       </c>
       <c r="M7" s="2">
-        <v>838591.639199998</v>
+        <v>2998146.3123999988</v>
       </c>
       <c r="N7" s="2">
-        <v>9.9999999999999591</v>
+        <v>21.99999999999995</v>
       </c>
       <c r="O7" s="2">
-        <v>251.99999999999952</v>
+        <v>1535</v>
       </c>
       <c r="P7" s="2">
-        <v>750105.80711999815</v>
+        <v>4597855.1592400009</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <v>25263.999999999989</v>
+        <v>22832.999999999989</v>
       </c>
       <c r="B8" s="2">
-        <v>4126.9999999999991</v>
+        <v>2624.9999999999973</v>
       </c>
       <c r="C8" s="3">
-        <v>20441.322639999999</v>
+        <v>19000.342280000001</v>
       </c>
       <c r="D8" s="2">
-        <v>17070.69999999999</v>
+        <v>12773.499999999993</v>
       </c>
       <c r="E8" s="2">
-        <v>27.999999999999929</v>
+        <v>480.99999999999943</v>
       </c>
       <c r="F8" s="2">
-        <v>268457.68935999984</v>
+        <v>477102.61020999961</v>
       </c>
       <c r="G8" s="3">
-        <v>21.79</v>
+        <v>32.450000000000003</v>
       </c>
       <c r="H8" s="2">
-        <v>73.999999999999488</v>
+        <v>83.999999999999417</v>
       </c>
       <c r="I8" s="2">
-        <v>69.999999999999687</v>
+        <v>66.999999999999702</v>
       </c>
       <c r="J8" s="2">
-        <v>202.59999999999971</v>
+        <v>586.09999999999911</v>
       </c>
       <c r="K8" s="2">
-        <v>314708.99999999988</v>
+        <v>13303.999999999976</v>
       </c>
       <c r="L8" s="2">
-        <v>18979.989999999991</v>
+        <v>31991.309999999979</v>
       </c>
       <c r="M8" s="2">
-        <v>3873762.5743999979</v>
+        <v>2339528.8654999975</v>
       </c>
       <c r="N8" s="2">
-        <v>28.999999999999932</v>
+        <v>40.999999999999879</v>
       </c>
       <c r="O8" s="2">
-        <v>1107.9999999999998</v>
+        <v>960.99999999999955</v>
       </c>
       <c r="P8" s="2">
-        <v>3584846.1060399981</v>
+        <v>507575.87836999819</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>17569.999999999989</v>
+        <v>15277.999999999991</v>
       </c>
       <c r="B9" s="2">
-        <v>1887.9999999999989</v>
+        <v>2241.9999999999986</v>
       </c>
       <c r="C9" s="2">
-        <v>18376.923200000001</v>
+        <v>18928.538</v>
       </c>
       <c r="D9" s="2">
-        <v>8486.1999999999953</v>
+        <v>5624.599999999994</v>
       </c>
       <c r="E9" s="2">
-        <v>234.99999999999972</v>
+        <v>253.99999999999974</v>
       </c>
       <c r="F9" s="2">
-        <v>341592.53969999967</v>
+        <v>305353.16715999978</v>
       </c>
       <c r="G9" s="2">
-        <v>26.3</v>
+        <v>28.41</v>
       </c>
       <c r="H9" s="2">
-        <v>155.99999999999895</v>
+        <v>54.999999999999609</v>
       </c>
       <c r="I9" s="2">
-        <v>56.999999999999723</v>
+        <v>34.999999999999837</v>
       </c>
       <c r="J9" s="2">
-        <v>389.39999999999952</v>
+        <v>982.89999999999884</v>
       </c>
       <c r="K9" s="2">
-        <v>182951.9999999998</v>
+        <v>22820.999999999982</v>
       </c>
       <c r="L9" s="2">
-        <v>19100.999999999978</v>
+        <v>13234.999999999989</v>
       </c>
       <c r="M9" s="2">
-        <v>2366184.0724999984</v>
+        <v>1244565.0463999989</v>
       </c>
       <c r="N9" s="2">
-        <v>24.999999999999932</v>
+        <v>24.999999999999929</v>
       </c>
       <c r="O9" s="2">
-        <v>790.99999999999943</v>
+        <v>693.99999999999932</v>
       </c>
       <c r="P9" s="2">
-        <v>322435.87408999965</v>
+        <v>3344506.7167999977</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>120926</v>
+        <v>9624.9999999999891</v>
       </c>
       <c r="B10" s="2">
-        <v>20037.999999999996</v>
+        <v>1255.9999999999986</v>
       </c>
       <c r="C10" s="2">
-        <v>25152.816680000011</v>
+        <v>16376.46312</v>
       </c>
       <c r="D10" s="2">
-        <v>72911.599999999991</v>
+        <v>6331.8999999999915</v>
       </c>
       <c r="E10" s="2">
-        <v>2549.9999999999977</v>
+        <v>135.99999999999977</v>
       </c>
       <c r="F10" s="2">
-        <v>4713511.9352799999</v>
+        <v>158372.48895999984</v>
       </c>
       <c r="G10" s="2">
-        <v>29.9</v>
+        <v>25.4</v>
       </c>
       <c r="H10" s="2">
-        <v>195.99999999999872</v>
+        <v>45.999999999999659</v>
       </c>
       <c r="I10" s="2">
-        <v>248.99999999999895</v>
+        <v>8.9999999999999467</v>
       </c>
       <c r="J10" s="2">
-        <v>1123.1999999999985</v>
+        <v>169.29999999999961</v>
       </c>
       <c r="K10" s="2">
-        <v>1264806.9999999993</v>
+        <v>61603.99999999992</v>
       </c>
       <c r="L10" s="2">
-        <v>104307.92999999998</v>
+        <v>13867.999999999985</v>
       </c>
       <c r="M10" s="2">
-        <v>2214641.3434399972</v>
+        <v>611275.27679999929</v>
       </c>
       <c r="N10" s="2">
-        <v>34.999999999999915</v>
+        <v>31.99999999999989</v>
       </c>
       <c r="O10" s="2">
-        <v>6308.9999999999991</v>
+        <v>405.99999999999937</v>
       </c>
       <c r="P10" s="2">
-        <v>26988496.705479994</v>
+        <v>85781.077479999847</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>50473.999999999993</v>
+        <v>7424.9999999999973</v>
       </c>
       <c r="B11" s="2">
-        <v>8680.9999999999982</v>
+        <v>1293</v>
       </c>
       <c r="C11" s="2">
-        <v>19397.3076</v>
+        <v>16443.209169999991</v>
       </c>
       <c r="D11" s="2">
-        <v>32935.899999999994</v>
+        <v>4607.6999999999971</v>
       </c>
       <c r="E11" s="2">
-        <v>1673.9999999999982</v>
+        <v>119.99999999999987</v>
       </c>
       <c r="F11" s="2">
-        <v>1330729.4930399999</v>
+        <v>219599.7193099999</v>
       </c>
       <c r="G11" s="2">
-        <v>25.1</v>
+        <v>27.9</v>
       </c>
       <c r="H11" s="2">
-        <v>158.99999999999895</v>
+        <v>20.999999999999858</v>
       </c>
       <c r="I11" s="2">
-        <v>184.99999999999918</v>
+        <v>17.999999999999915</v>
       </c>
       <c r="J11" s="2">
-        <v>386.19999999999953</v>
+        <v>153.79999999999984</v>
       </c>
       <c r="K11" s="2">
-        <v>810919.99999999977</v>
+        <v>16620.999999999989</v>
       </c>
       <c r="L11" s="2">
-        <v>182696</v>
+        <v>11932.299999999996</v>
       </c>
       <c r="M11" s="2">
-        <v>5519372.8535999991</v>
+        <v>742537.84159999969</v>
       </c>
       <c r="N11" s="2">
-        <v>38.999999999999908</v>
+        <v>14.999999999999963</v>
       </c>
       <c r="O11" s="2">
-        <v>2499.9999999999995</v>
+        <v>440.99999999999977</v>
       </c>
       <c r="P11" s="2">
-        <v>3749387.5015199976</v>
+        <v>123348.75611999938</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>23671.999999999989</v>
+        <v>4183.9999999999918</v>
       </c>
       <c r="B12" s="2">
-        <v>2819.9999999999991</v>
+        <v>788.99999999999841</v>
       </c>
       <c r="C12" s="2">
-        <v>17545.93204</v>
+        <v>19068.8688</v>
       </c>
       <c r="D12" s="2">
-        <v>16399.19999999999</v>
+        <v>1820.9999999999964</v>
       </c>
       <c r="E12" s="2">
-        <v>346.9999999999996</v>
+        <v>79.999999999999787</v>
       </c>
       <c r="F12" s="2">
-        <v>573514.04293999996</v>
+        <v>57968.611199999868</v>
       </c>
       <c r="G12" s="2">
-        <v>28</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="H12" s="2">
-        <v>64.999999999999574</v>
+        <v>12.999999999999892</v>
       </c>
       <c r="I12" s="2">
-        <v>59.999999999999716</v>
+        <v>1.9999999999999847</v>
       </c>
       <c r="J12" s="2">
-        <v>382.49999999999949</v>
+        <v>81.399999999999764</v>
       </c>
       <c r="K12" s="2">
-        <v>39639.999999999935</v>
+        <v>32010.999999999935</v>
       </c>
       <c r="L12" s="2">
-        <v>9314.3999999999924</v>
+        <v>1244.4599999999969</v>
       </c>
       <c r="M12" s="2">
-        <v>3234408.7671999987</v>
+        <v>838591.639199998</v>
       </c>
       <c r="N12" s="2">
-        <v>17.99999999999995</v>
+        <v>9.9999999999999591</v>
       </c>
       <c r="O12" s="2">
-        <v>744.99999999999955</v>
+        <v>251.99999999999952</v>
       </c>
       <c r="P12" s="2">
-        <v>828015.21829999797</v>
+        <v>750105.80711999815</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>116468</v>
+        <v>25263.999999999989</v>
       </c>
       <c r="B13" s="2">
-        <v>21239.000000000004</v>
+        <v>4126.9999999999991</v>
       </c>
       <c r="C13" s="2">
-        <v>23604.910929999998</v>
+        <v>20441.322639999999</v>
       </c>
       <c r="D13" s="2">
-        <v>64664.399999999987</v>
+        <v>17070.69999999999</v>
       </c>
       <c r="E13" s="2">
-        <v>2076.9999999999995</v>
+        <v>27.999999999999929</v>
       </c>
       <c r="F13" s="2">
-        <v>4676977.1911800001</v>
+        <v>268457.68935999984</v>
       </c>
       <c r="G13" s="2">
-        <v>30.2</v>
+        <v>21.79</v>
       </c>
       <c r="H13" s="2">
-        <v>300.99999999999807</v>
+        <v>73.999999999999488</v>
       </c>
       <c r="I13" s="2">
-        <v>303.99999999999869</v>
+        <v>69.999999999999687</v>
       </c>
       <c r="J13" s="2">
-        <v>783.79999999999882</v>
+        <v>202.59999999999971</v>
       </c>
       <c r="K13" s="2">
-        <v>202571.00000000003</v>
+        <v>314708.99999999988</v>
       </c>
       <c r="L13" s="2">
-        <v>87368.909999999974</v>
+        <v>18979.989999999991</v>
       </c>
       <c r="M13" s="2">
-        <v>8408723.8795999978</v>
+        <v>3873762.5743999979</v>
       </c>
       <c r="N13" s="2">
-        <v>34.999999999999901</v>
+        <v>28.999999999999932</v>
       </c>
       <c r="O13" s="2">
-        <v>4502</v>
+        <v>1107.9999999999998</v>
       </c>
       <c r="P13" s="2">
-        <v>19397519.885310002</v>
+        <v>3584846.1060399981</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>64841.999999999993</v>
+        <v>17569.999999999989</v>
       </c>
       <c r="B14" s="2">
-        <v>15028.999999999996</v>
+        <v>1887.9999999999989</v>
       </c>
       <c r="C14" s="2">
-        <v>25869.387780000001</v>
+        <v>18376.923200000001</v>
       </c>
       <c r="D14" s="2">
-        <v>17235.499999999989</v>
+        <v>8486.1999999999953</v>
       </c>
       <c r="E14" s="2">
-        <v>1123.9999999999986</v>
+        <v>234.99999999999972</v>
       </c>
       <c r="F14" s="2">
-        <v>866008.93850999954</v>
+        <v>341592.53969999967</v>
       </c>
       <c r="G14" s="2">
-        <v>23.8</v>
+        <v>26.3</v>
       </c>
       <c r="H14" s="2">
-        <v>124.99999999999919</v>
+        <v>155.99999999999895</v>
       </c>
       <c r="I14" s="2">
-        <v>194.99999999999915</v>
+        <v>56.999999999999723</v>
       </c>
       <c r="J14" s="2">
-        <v>235.39999999999975</v>
+        <v>389.39999999999952</v>
       </c>
       <c r="K14" s="2">
-        <v>2168.999999999995</v>
+        <v>182951.9999999998</v>
       </c>
       <c r="L14" s="2">
-        <v>22439.059999999987</v>
+        <v>19100.999999999978</v>
       </c>
       <c r="M14" s="2">
-        <v>259751.15039999882</v>
+        <v>2366184.0724999984</v>
       </c>
       <c r="N14" s="2">
-        <v>11.999999999999948</v>
+        <v>24.999999999999932</v>
       </c>
       <c r="O14" s="2">
-        <v>3210.9999999999995</v>
+        <v>790.99999999999943</v>
       </c>
       <c r="P14" s="2">
-        <v>9430951.7147999946</v>
+        <v>322435.87408999965</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>64100</v>
+        <v>120926</v>
       </c>
       <c r="B15" s="2">
-        <v>9192</v>
+        <v>20037.999999999996</v>
       </c>
       <c r="C15" s="2">
-        <v>21205.026720000002</v>
+        <v>25152.816680000011</v>
       </c>
       <c r="D15" s="2">
-        <v>59994</v>
+        <v>72911.599999999991</v>
       </c>
       <c r="E15" s="2">
-        <v>1042.9999999999993</v>
+        <v>2549.9999999999977</v>
       </c>
       <c r="F15" s="2">
-        <v>1194600.3487199994</v>
+        <v>4713511.9352799999</v>
       </c>
       <c r="G15" s="2">
-        <v>24.81</v>
+        <v>29.9</v>
       </c>
       <c r="H15" s="2">
-        <v>140.99999999999912</v>
+        <v>195.99999999999872</v>
       </c>
       <c r="I15" s="2">
-        <v>92.999999999999559</v>
+        <v>248.99999999999895</v>
       </c>
       <c r="J15" s="2">
-        <v>563.59999999999923</v>
+        <v>1123.1999999999985</v>
       </c>
       <c r="K15" s="2">
-        <v>35895.999999999993</v>
+        <v>1264806.9999999993</v>
       </c>
       <c r="L15" s="2">
-        <v>57654.419999999991</v>
+        <v>104307.92999999998</v>
       </c>
       <c r="M15" s="2">
-        <v>8271274.1760000018</v>
+        <v>2214641.3434399972</v>
       </c>
       <c r="N15" s="2">
-        <v>36.999999999999908</v>
+        <v>34.999999999999915</v>
       </c>
       <c r="O15" s="2">
-        <v>3089.9999999999995</v>
+        <v>6308.9999999999991</v>
       </c>
       <c r="P15" s="2">
-        <v>7029925.2345599988</v>
+        <v>26988496.705479994</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>105038</v>
+        <v>50473.999999999993</v>
       </c>
       <c r="B16" s="2">
-        <v>11442</v>
+        <v>8680.9999999999982</v>
       </c>
       <c r="C16" s="2">
-        <v>18218.315640000001</v>
+        <v>19397.3076</v>
       </c>
       <c r="D16" s="2">
-        <v>69421.599999999991</v>
+        <v>32935.899999999994</v>
       </c>
       <c r="E16" s="2">
-        <v>79.999999999999517</v>
+        <v>1673.9999999999982</v>
       </c>
       <c r="F16" s="2">
-        <v>3389505.0556999999</v>
+        <v>1330729.4930399999</v>
       </c>
       <c r="G16" s="2">
-        <v>21.85</v>
+        <v>25.1</v>
       </c>
       <c r="H16" s="2">
-        <v>164.99999999999895</v>
+        <v>158.99999999999895</v>
       </c>
       <c r="I16" s="2">
-        <v>248.99999999999898</v>
+        <v>184.99999999999918</v>
       </c>
       <c r="J16" s="2">
-        <v>369.09999999999923</v>
+        <v>386.19999999999953</v>
       </c>
       <c r="K16" s="2">
-        <v>18256.999999999818</v>
+        <v>810919.99999999977</v>
       </c>
       <c r="L16" s="2">
-        <v>57789.999999999949</v>
+        <v>182696</v>
       </c>
       <c r="M16" s="2">
-        <v>521260.11459999764</v>
+        <v>5519372.8535999991</v>
       </c>
       <c r="N16" s="2">
-        <v>5.9999999999999627</v>
+        <v>38.999999999999908</v>
       </c>
       <c r="O16" s="2">
-        <v>3403</v>
+        <v>2499.9999999999995</v>
       </c>
       <c r="P16" s="2">
-        <v>5939939.1027600002</v>
+        <v>3749387.5015199976</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>9622.9999999999964</v>
+        <v>8854.9999999999945</v>
       </c>
       <c r="B17" s="2">
-        <v>2088.3249137487501</v>
+        <v>1278.9999999999998</v>
       </c>
       <c r="C17" s="2">
-        <v>19210.228831246099</v>
+        <v>2585.4999999999986</v>
       </c>
       <c r="D17" s="2">
-        <v>3746.5999999999972</v>
+        <v>281.99999999999972</v>
       </c>
       <c r="E17" s="2">
-        <v>44.99999999999995</v>
+        <v>415783.74875999975</v>
       </c>
       <c r="F17" s="2">
-        <v>84821.616612874292</v>
+        <v>46.954686477696221</v>
       </c>
       <c r="G17" s="2">
-        <v>35.438037383177502</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="H17" s="2">
-        <v>54.072514242661697</v>
+        <v>16.999999999999883</v>
       </c>
       <c r="I17" s="2">
-        <v>9.9999999999999485</v>
+        <v>15.999999999999924</v>
       </c>
       <c r="J17" s="2">
-        <v>220.54621652251561</v>
+        <v>410.99999999999943</v>
       </c>
       <c r="K17" s="2">
-        <v>32749.978346102071</v>
+        <v>89147.199999999983</v>
       </c>
       <c r="L17" s="2">
-        <v>14259.056285147481</v>
+        <v>7671.9999999999945</v>
       </c>
       <c r="M17" s="2">
-        <v>633508.48902710096</v>
+        <v>2684633.8327999976</v>
       </c>
       <c r="N17" s="2">
-        <v>22.70687713300876</v>
+        <v>18.999999999999947</v>
       </c>
       <c r="O17" s="2">
-        <v>672.99999999999989</v>
+        <v>376.99999999999977</v>
       </c>
       <c r="P17" s="2">
-        <v>286032.99613732687</v>
+        <v>366113.43699999945</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>16685</v>
+        <v>17833.999999999989</v>
       </c>
       <c r="B18" s="2">
-        <v>2386</v>
+        <v>2086.9999999999986</v>
       </c>
       <c r="C18" s="2">
-        <v>19210.228831246099</v>
+        <v>6433.2999999999956</v>
       </c>
       <c r="D18" s="2">
-        <v>10592.2</v>
+        <v>210.99999999999983</v>
       </c>
       <c r="E18" s="2">
-        <v>377.99999999999972</v>
+        <v>267414.72803999996</v>
       </c>
       <c r="F18" s="2">
-        <v>398404.10684000002</v>
+        <v>14.994657846809471</v>
       </c>
       <c r="G18" s="2">
-        <v>35.438037383177502</v>
+        <v>32.08</v>
       </c>
       <c r="H18" s="2">
-        <v>54.072514242661697</v>
+        <v>84.999999999999403</v>
       </c>
       <c r="I18" s="2">
-        <v>28.221234650144272</v>
+        <v>54.999999999999737</v>
       </c>
       <c r="J18" s="2">
-        <v>800.99999999999955</v>
+        <v>537.09999999999934</v>
       </c>
       <c r="K18" s="2">
-        <v>112137</v>
+        <v>297093.99999999983</v>
       </c>
       <c r="L18" s="2">
-        <v>14259.056285147481</v>
+        <v>16965.999999999989</v>
       </c>
       <c r="M18" s="2">
-        <v>1610842.1836000001</v>
+        <v>2513116.4799999981</v>
       </c>
       <c r="N18" s="2">
-        <v>22.70687713300876</v>
+        <v>39.999999999999886</v>
       </c>
       <c r="O18" s="2">
-        <v>624.00000000000011</v>
+        <v>810.99999999999943</v>
       </c>
       <c r="P18" s="2">
-        <v>1492496.0792400001</v>
+        <v>1568477.3210399991</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>40956</v>
+        <v>22243.999999999989</v>
       </c>
       <c r="B19" s="2">
-        <v>6906.9999999999973</v>
+        <v>2688.9999999999995</v>
       </c>
       <c r="C19" s="2">
-        <v>19210.228831246099</v>
+        <v>9015.3999999999905</v>
       </c>
       <c r="D19" s="2">
-        <v>45679.399999999987</v>
+        <v>204.99999999999977</v>
       </c>
       <c r="E19" s="2">
-        <v>943.99999999999955</v>
+        <v>229243.99999999988</v>
       </c>
       <c r="F19" s="2">
-        <v>1135992.2059200001</v>
+        <v>10.305880237367379</v>
       </c>
       <c r="G19" s="2">
-        <v>35.438037383177502</v>
+        <v>21.93</v>
       </c>
       <c r="H19" s="2">
-        <v>86.999999999999389</v>
+        <v>70.999999999999531</v>
       </c>
       <c r="I19" s="2">
-        <v>196.9999999999992</v>
+        <v>30.999999999999837</v>
       </c>
       <c r="J19" s="2">
-        <v>2450.9999999999991</v>
+        <v>98.599999999999739</v>
       </c>
       <c r="K19" s="2">
-        <v>49269.999999999927</v>
+        <v>279415.99999999988</v>
       </c>
       <c r="L19" s="2">
-        <v>14259.056285147481</v>
+        <v>4925.9999999999973</v>
       </c>
       <c r="M19" s="2">
-        <v>1321756.1130112109</v>
+        <v>3402333.9999999972</v>
       </c>
       <c r="N19" s="2">
-        <v>26.99999999999994</v>
+        <v>20.999999999999943</v>
       </c>
       <c r="O19" s="2">
-        <v>1960</v>
+        <v>978.9999999999992</v>
       </c>
       <c r="P19" s="2">
-        <v>1961160.027659998</v>
+        <v>602011.49999999895</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <v>24184.999999999989</v>
+        <v>35142.999999999993</v>
       </c>
       <c r="B20" s="2">
-        <v>4568.9999999999982</v>
+        <v>4696.9999999999991</v>
       </c>
       <c r="C20" s="2">
-        <v>21418.87329</v>
+        <v>27639.699999999986</v>
       </c>
       <c r="D20" s="2">
-        <v>7762.6753209116032</v>
+        <v>219.99999999999972</v>
       </c>
       <c r="E20" s="2">
-        <v>130.9999999999998</v>
+        <v>794230.03655999957</v>
       </c>
       <c r="F20" s="2">
-        <v>153719.09000888691</v>
+        <v>22.599949821016981</v>
       </c>
       <c r="G20" s="2">
-        <v>35.438037383177502</v>
+        <v>22.85</v>
       </c>
       <c r="H20" s="2">
-        <v>103.9999999999993</v>
+        <v>125.9999999999992</v>
       </c>
       <c r="I20" s="2">
-        <v>2.999999999999976</v>
+        <v>95.999999999999559</v>
       </c>
       <c r="J20" s="2">
-        <v>479.14656225630722</v>
+        <v>536.7999999999995</v>
       </c>
       <c r="K20" s="2">
-        <v>106498</v>
+        <v>378688.00000000006</v>
       </c>
       <c r="L20" s="2">
-        <v>19137.909999999989</v>
+        <v>9071.9999999999927</v>
       </c>
       <c r="M20" s="2">
-        <v>3427876.6054999982</v>
+        <v>8906174.1647999976</v>
       </c>
       <c r="N20" s="2">
-        <v>50.999999999999893</v>
+        <v>18.999999999999954</v>
       </c>
       <c r="O20" s="2">
-        <v>1218</v>
+        <v>1432.9999999999993</v>
       </c>
       <c r="P20" s="2">
-        <v>3524494.8488999992</v>
+        <v>3135363.9667199976</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <v>12565.999999999991</v>
+        <v>31885.999999999989</v>
       </c>
       <c r="B21" s="2">
-        <v>2093.9999999999991</v>
+        <v>5471</v>
       </c>
       <c r="C21" s="2">
-        <v>19210.228831246099</v>
+        <v>9993.7999999999938</v>
       </c>
       <c r="D21" s="2">
-        <v>7762.6753209116032</v>
+        <v>349.99999999999949</v>
       </c>
       <c r="E21" s="2">
-        <v>449.99999999999937</v>
+        <v>135007.86686999991</v>
       </c>
       <c r="F21" s="2">
-        <v>374829.37895564421</v>
+        <v>4.2340797487925723</v>
       </c>
       <c r="G21" s="2">
-        <v>35.438037383177502</v>
+        <v>22.88</v>
       </c>
       <c r="H21" s="2">
-        <v>59.999999999999581</v>
+        <v>126.99999999999916</v>
       </c>
       <c r="I21" s="2">
-        <v>28.221234650144272</v>
+        <v>24.999999999999879</v>
       </c>
       <c r="J21" s="2">
-        <v>647.79999999999916</v>
+        <v>357.59999999999962</v>
       </c>
       <c r="K21" s="2">
-        <v>32749.978346102071</v>
+        <v>532404</v>
       </c>
       <c r="L21" s="2">
-        <v>20804.14999999998</v>
+        <v>27023.969999999979</v>
       </c>
       <c r="M21" s="2">
-        <v>1533618.0888999989</v>
+        <v>9174521.0092999972</v>
       </c>
       <c r="N21" s="2">
-        <v>22.70687713300876</v>
+        <v>29.999999999999922</v>
       </c>
       <c r="O21" s="2">
-        <v>676.99999999999955</v>
+        <v>2096.9999999999995</v>
       </c>
       <c r="P21" s="2">
-        <v>1868542.2159599981</v>
+        <v>17566777.100189991</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <v>4183.9999999999918</v>
+        <v>23671.999999999989</v>
       </c>
       <c r="B22" s="2">
-        <v>1056.473753859249</v>
+        <v>2819.9999999999991</v>
       </c>
       <c r="C22" s="2">
-        <v>20427.341848341399</v>
+        <v>17545.93204</v>
       </c>
       <c r="D22" s="2">
-        <v>2381.065679515827</v>
+        <v>16399.19999999999</v>
       </c>
       <c r="E22" s="2">
-        <v>113.4249949517034</v>
+        <v>346.9999999999996</v>
       </c>
       <c r="F22" s="2">
-        <v>81501.246245260627</v>
+        <v>573514.04293999996</v>
       </c>
       <c r="G22" s="2">
-        <v>35.799999999999997</v>
+        <v>28</v>
       </c>
       <c r="H22" s="2">
-        <v>15.982526713303701</v>
+        <v>64.999999999999574</v>
       </c>
       <c r="I22" s="2">
-        <v>2.5736340998794449</v>
+        <v>59.999999999999716</v>
       </c>
       <c r="J22" s="2">
-        <v>109.9937054332045</v>
+        <v>382.49999999999949</v>
       </c>
       <c r="K22" s="2">
-        <v>44335.913688073488</v>
+        <v>39639.999999999935</v>
       </c>
       <c r="L22" s="2">
-        <v>2003.2628205799081</v>
+        <v>9314.3999999999924</v>
       </c>
       <c r="M22" s="2">
-        <v>1077875.2283725089</v>
+        <v>3234408.7671999987</v>
       </c>
       <c r="N22" s="2">
-        <v>11.577914620948469</v>
+        <v>17.99999999999995</v>
       </c>
       <c r="O22" s="2">
-        <v>315.84662311287587</v>
+        <v>744.99999999999955</v>
       </c>
       <c r="P22" s="2">
-        <v>1122077.8321941849</v>
+        <v>828015.21829999797</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>25263.999999999989</v>
+        <v>116468</v>
       </c>
       <c r="B23" s="2">
-        <v>5714.5080545330657</v>
+        <v>21239.000000000004</v>
       </c>
       <c r="C23" s="2">
-        <v>20441.322639999999</v>
+        <v>23604.910929999998</v>
       </c>
       <c r="D23" s="2">
-        <v>18620.078602856651</v>
+        <v>64664.399999999987</v>
       </c>
       <c r="E23" s="2">
-        <v>39.698748233096183</v>
+        <v>2076.9999999999995</v>
       </c>
       <c r="F23" s="2">
-        <v>377439.37268869882</v>
+        <v>4676977.1911800001</v>
       </c>
       <c r="G23" s="2">
-        <v>28.859170731707302</v>
+        <v>30.2</v>
       </c>
       <c r="H23" s="2">
-        <v>121.2195445843775</v>
+        <v>300.99999999999807</v>
       </c>
       <c r="I23" s="2">
-        <v>82.574144705994001</v>
+        <v>303.99999999999869</v>
       </c>
       <c r="J23" s="2">
-        <v>273.76811696274279</v>
+        <v>783.79999999999882</v>
       </c>
       <c r="K23" s="2">
-        <v>390629.37411319528</v>
+        <v>202571.00000000003</v>
       </c>
       <c r="L23" s="2">
-        <v>30552.937259516999</v>
+        <v>87368.909999999974</v>
       </c>
       <c r="M23" s="2">
-        <v>5170690.3577637998</v>
+        <v>8408723.8795999978</v>
       </c>
       <c r="N23" s="2">
-        <v>37.037791832750607</v>
+        <v>34.999999999999901</v>
       </c>
       <c r="O23" s="2">
-        <v>1578.0387530220919</v>
+        <v>4502</v>
       </c>
       <c r="P23" s="2">
-        <v>5162046.5029202029</v>
+        <v>19397519.885310002</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <v>17569.999999999989</v>
+        <v>64841.999999999993</v>
       </c>
       <c r="B24" s="2">
-        <v>2528.0385897164319</v>
+        <v>15028.999999999996</v>
       </c>
       <c r="C24" s="2">
-        <v>20427.341848341399</v>
+        <v>25869.387780000001</v>
       </c>
       <c r="D24" s="2">
-        <v>11096.210636742029</v>
+        <v>17235.499999999989</v>
       </c>
       <c r="E24" s="2">
-        <v>333.18592267062911</v>
+        <v>1123.9999999999986</v>
       </c>
       <c r="F24" s="2">
-        <v>480263.66540990549</v>
+        <v>866008.93850999954</v>
       </c>
       <c r="G24" s="2">
-        <v>28.859170731707302</v>
+        <v>23.8</v>
       </c>
       <c r="H24" s="2">
-        <v>155.99999999999889</v>
+        <v>124.99999999999919</v>
       </c>
       <c r="I24" s="2">
-        <v>82.574144705994001</v>
+        <v>194.99999999999915</v>
       </c>
       <c r="J24" s="2">
-        <v>675.1104937785783</v>
+        <v>235.39999999999975</v>
       </c>
       <c r="K24" s="2">
-        <v>253392.3988960179</v>
+        <v>2168.999999999995</v>
       </c>
       <c r="L24" s="2">
-        <v>30747.732458975679</v>
+        <v>22439.059999999987</v>
       </c>
       <c r="M24" s="2">
-        <v>3041350.614883801</v>
+        <v>259751.15039999882</v>
       </c>
       <c r="N24" s="2">
-        <v>37.037791832750607</v>
+        <v>11.999999999999948</v>
       </c>
       <c r="O24" s="2">
-        <v>1578.0387530220919</v>
+        <v>3210.9999999999995</v>
       </c>
       <c r="P24" s="2">
-        <v>482329.48363598721</v>
+        <v>9430951.7147999946</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <v>120926</v>
+        <v>64100</v>
       </c>
       <c r="B25" s="2">
-        <v>20038</v>
+        <v>9192</v>
       </c>
       <c r="C25" s="2">
-        <v>25152.816680000011</v>
+        <v>21205.026720000002</v>
       </c>
       <c r="D25" s="2">
-        <v>72911.599999999991</v>
+        <v>59994</v>
       </c>
       <c r="E25" s="2">
-        <v>2549.9999999999982</v>
+        <v>1042.9999999999993</v>
       </c>
       <c r="F25" s="2">
-        <v>4713511.9352799999</v>
+        <v>1194600.3487199994</v>
       </c>
       <c r="G25" s="2">
-        <v>29.9</v>
+        <v>24.81</v>
       </c>
       <c r="H25" s="2">
-        <v>195.99999999999869</v>
+        <v>140.99999999999912</v>
       </c>
       <c r="I25" s="2">
-        <v>248.99999999999889</v>
+        <v>92.999999999999559</v>
       </c>
       <c r="J25" s="2">
-        <v>1123.199999999998</v>
+        <v>563.59999999999923</v>
       </c>
       <c r="K25" s="2">
-        <v>1264806.9999999991</v>
+        <v>35895.999999999993</v>
       </c>
       <c r="L25" s="2">
-        <v>104307.93</v>
+        <v>57654.419999999991</v>
       </c>
       <c r="M25" s="2">
-        <v>2846566.7104680962</v>
+        <v>8271274.1760000018</v>
       </c>
       <c r="N25" s="2">
-        <v>37.037791832750607</v>
+        <v>36.999999999999908</v>
       </c>
       <c r="O25" s="2">
-        <v>6308.9999999999991</v>
+        <v>3089.9999999999995</v>
       </c>
       <c r="P25" s="2">
-        <v>26988496.705479991</v>
+        <v>7029925.2345599988</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <v>50473.999999999993</v>
+        <v>105038</v>
       </c>
       <c r="B26" s="2">
-        <v>8680.9999999999982</v>
+        <v>11442</v>
       </c>
       <c r="C26" s="2">
-        <v>20427.341848341399</v>
+        <v>18218.315640000001</v>
       </c>
       <c r="D26" s="2">
-        <v>32935.899999999987</v>
+        <v>69421.599999999991</v>
       </c>
       <c r="E26" s="2">
-        <v>1673.999999999998</v>
+        <v>79.999999999999517</v>
       </c>
       <c r="F26" s="2">
-        <v>1330729.4930400001</v>
+        <v>3389505.0556999999</v>
       </c>
       <c r="G26" s="2">
-        <v>28.859170731707302</v>
+        <v>21.85</v>
       </c>
       <c r="H26" s="2">
-        <v>158.99999999999889</v>
+        <v>164.99999999999895</v>
       </c>
       <c r="I26" s="2">
-        <v>184.9999999999992</v>
+        <v>248.99999999999898</v>
       </c>
       <c r="J26" s="2">
-        <v>675.1104937785783</v>
+        <v>369.09999999999923</v>
       </c>
       <c r="K26" s="2">
-        <v>810919.99999999977</v>
+        <v>18256.999999999818</v>
       </c>
       <c r="L26" s="2">
-        <v>182696</v>
+        <v>57789.999999999949</v>
       </c>
       <c r="M26" s="2">
-        <v>5519372.8535999991</v>
+        <v>521260.11459999764</v>
       </c>
       <c r="N26" s="2">
-        <v>38.999999999999908</v>
+        <v>5.9999999999999627</v>
       </c>
       <c r="O26" s="2">
-        <v>2500</v>
+        <v>3403</v>
       </c>
       <c r="P26" s="2">
-        <v>5162046.5029202029</v>
+        <v>5939939.1027600002</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
-        <v>23671.999999999989</v>
+        <v>22677.999999999989</v>
       </c>
       <c r="B27" s="2">
-        <v>5316.1026797151171</v>
+        <v>2547.9999999999977</v>
       </c>
       <c r="C27" s="2">
-        <v>20804.770158470299</v>
+        <v>18638.87111</v>
       </c>
       <c r="D27" s="2">
-        <v>18102.33886557139</v>
+        <v>10254.999999999993</v>
       </c>
       <c r="E27" s="2">
-        <v>692.21862862467367</v>
+        <v>511.99999999999943</v>
       </c>
       <c r="F27" s="2">
-        <v>786293.0504705467</v>
+        <v>451466.86220999988</v>
       </c>
       <c r="G27" s="2">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H27" s="2">
-        <v>90.463582676213051</v>
+        <v>83.999999999999432</v>
       </c>
       <c r="I27" s="2">
-        <v>70.480699544079414</v>
+        <v>32.999999999999851</v>
       </c>
       <c r="J27" s="2">
-        <v>497.85288158683818</v>
+        <v>265.79999999999973</v>
       </c>
       <c r="K27" s="2">
-        <v>61373.672326328422</v>
+        <v>14455.999999999975</v>
       </c>
       <c r="L27" s="2">
-        <v>12579.47779916077</v>
+        <v>35901.049999999996</v>
       </c>
       <c r="M27" s="2">
-        <v>3234408.7671999992</v>
+        <v>1395103.6922999984</v>
       </c>
       <c r="N27" s="2">
-        <v>28.514194264827129</v>
+        <v>25.999999999999936</v>
       </c>
       <c r="O27" s="2">
-        <v>801.10415672385136</v>
+        <v>919.99999999999955</v>
       </c>
       <c r="P27" s="2">
-        <v>1155335.2855618461</v>
+        <v>932526.86903999816</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
-        <v>116468</v>
+        <v>17174.999999999989</v>
       </c>
       <c r="B28" s="2">
-        <v>21239</v>
+        <v>2330.9999999999977</v>
       </c>
       <c r="C28" s="2">
-        <v>23604.910929999998</v>
+        <v>22823.19152</v>
       </c>
       <c r="D28" s="2">
-        <v>64664.399999999987</v>
+        <v>6715.4999999999927</v>
       </c>
       <c r="E28" s="2">
-        <v>2077</v>
+        <v>244.99999999999955</v>
       </c>
       <c r="F28" s="2">
-        <v>4676977.1911799992</v>
+        <v>235832.72977999973</v>
       </c>
       <c r="G28" s="2">
-        <v>30.2</v>
+        <v>27.3</v>
       </c>
       <c r="H28" s="2">
-        <v>300.99999999999812</v>
+        <v>76.99999999999946</v>
       </c>
       <c r="I28" s="2">
-        <v>303.99999999999869</v>
+        <v>7.9999999999999538</v>
       </c>
       <c r="J28" s="2">
-        <v>783.79999999999882</v>
+        <v>81.299999999999784</v>
       </c>
       <c r="K28" s="2">
-        <v>202571</v>
+        <v>86576.999999999913</v>
       </c>
       <c r="L28" s="2">
-        <v>87368.909999999974</v>
+        <v>15944.749999999989</v>
       </c>
       <c r="M28" s="2">
-        <v>8408723.8795999978</v>
+        <v>1820784.7858999991</v>
       </c>
       <c r="N28" s="2">
-        <v>34.999999999999901</v>
+        <v>15.99999999999995</v>
       </c>
       <c r="O28" s="2">
-        <v>4502</v>
+        <v>729.99999999999955</v>
       </c>
       <c r="P28" s="2">
-        <v>19397519.885310002</v>
+        <v>1460779.4436599989</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <v>64841.999999999993</v>
+        <v>39066.999999999993</v>
       </c>
       <c r="B29" s="2">
-        <v>15029</v>
+        <v>6011.9999999999982</v>
       </c>
       <c r="C29" s="2">
-        <v>25869.387780000001</v>
+        <v>18611.958289999999</v>
       </c>
       <c r="D29" s="2">
-        <v>18102.33886557139</v>
+        <v>20455.999999999993</v>
       </c>
       <c r="E29" s="2">
-        <v>1123.9999999999991</v>
+        <v>645.99999999999943</v>
       </c>
       <c r="F29" s="2">
-        <v>866008.93850999954</v>
+        <v>899043.39099999995</v>
       </c>
       <c r="G29" s="2">
-        <v>26.112401315789398</v>
+        <v>37.19</v>
       </c>
       <c r="H29" s="2">
-        <v>124.9999999999992</v>
+        <v>147.99999999999906</v>
       </c>
       <c r="I29" s="2">
-        <v>194.99999999999909</v>
+        <v>40.999999999999794</v>
       </c>
       <c r="J29" s="2">
-        <v>257.87557539933027</v>
+        <v>618.49999999999932</v>
       </c>
       <c r="K29" s="2">
-        <v>2327.949027416018</v>
+        <v>27023.999999999942</v>
       </c>
       <c r="L29" s="2">
-        <v>29602.9087374105</v>
+        <v>26455.999999999993</v>
       </c>
       <c r="M29" s="2">
-        <v>352889.09448255628</v>
+        <v>2652645.5177999986</v>
       </c>
       <c r="N29" s="2">
-        <v>11.99999999999995</v>
+        <v>18.99999999999995</v>
       </c>
       <c r="O29" s="2">
-        <v>3211</v>
+        <v>1149.9999999999995</v>
       </c>
       <c r="P29" s="2">
-        <v>9430951.7147999946</v>
+        <v>6067714.9468499981</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <v>64100</v>
+        <v>27626.999999999989</v>
       </c>
       <c r="B30" s="2">
-        <v>9192</v>
+        <v>3520.9999999999991</v>
       </c>
       <c r="C30" s="2">
-        <v>21205.026720000002</v>
+        <v>19147.145039999999</v>
       </c>
       <c r="D30" s="2">
-        <v>59994</v>
+        <v>11267.999999999993</v>
       </c>
       <c r="E30" s="2">
-        <v>1042.9999999999991</v>
+        <v>1097.9999999999991</v>
       </c>
       <c r="F30" s="2">
-        <v>1194600.348719999</v>
+        <v>584236.91447999945</v>
       </c>
       <c r="G30" s="2">
-        <v>26.112401315789398</v>
+        <v>51.2</v>
       </c>
       <c r="H30" s="2">
-        <v>140.99999999999909</v>
+        <v>122.99999999999919</v>
       </c>
       <c r="I30" s="2">
-        <v>92.999999999999559</v>
+        <v>36.999999999999829</v>
       </c>
       <c r="J30" s="2">
-        <v>563.59999999999923</v>
+        <v>408.3999999999993</v>
       </c>
       <c r="K30" s="2">
-        <v>61373.672326328422</v>
+        <v>38837.999999999964</v>
       </c>
       <c r="L30" s="2">
-        <v>57654.419999999991</v>
+        <v>26779.999999999989</v>
       </c>
       <c r="M30" s="2">
-        <v>8271274.1760000018</v>
+        <v>2725337.6207999978</v>
       </c>
       <c r="N30" s="2">
-        <v>36.999999999999908</v>
+        <v>16.999999999999954</v>
       </c>
       <c r="O30" s="2">
-        <v>3090</v>
+        <v>1043.9999999999995</v>
       </c>
       <c r="P30" s="2">
-        <v>7029925.2345599988</v>
+        <v>556306.09055999748</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <v>105038</v>
+        <v>31271</v>
       </c>
       <c r="B31" s="2">
-        <v>11442</v>
+        <v>4769.9999999999982</v>
       </c>
       <c r="C31" s="2">
-        <v>20804.770158470299</v>
+        <v>16996.987359999999</v>
       </c>
       <c r="D31" s="2">
-        <v>69421.599999999991</v>
+        <v>11655.999999999998</v>
       </c>
       <c r="E31" s="2">
-        <v>104.0508328856842</v>
+        <v>633.99999999999977</v>
       </c>
       <c r="F31" s="2">
-        <v>3389505.0557000008</v>
+        <v>312410.58597000001</v>
       </c>
       <c r="G31" s="2">
-        <v>26.112401315789398</v>
+        <v>29.58</v>
       </c>
       <c r="H31" s="2">
-        <v>164.99999999999889</v>
+        <v>71.999999999999559</v>
       </c>
       <c r="I31" s="2">
-        <v>248.99999999999901</v>
+        <v>113.99999999999952</v>
       </c>
       <c r="J31" s="2">
-        <v>497.85288158683818</v>
+        <v>478.49999999999966</v>
       </c>
       <c r="K31" s="2">
-        <v>19594.912583464229</v>
+        <v>116217.99999999997</v>
       </c>
       <c r="L31" s="2">
-        <v>57789.999999999949</v>
+        <v>29804.749999999989</v>
       </c>
       <c r="M31" s="2">
-        <v>708166.29511669534</v>
+        <v>5228156.3358999994</v>
       </c>
       <c r="N31" s="2">
-        <v>5.9999999999999627</v>
+        <v>38.999999999999915</v>
       </c>
       <c r="O31" s="2">
-        <v>3403</v>
+        <v>1186.9999999999998</v>
       </c>
       <c r="P31" s="2">
-        <v>5939939.1027599983</v>
+        <v>2895385.0253199995</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -1974,49 +1974,49 @@
         <v>9622.9999999999964</v>
       </c>
       <c r="B32" s="2">
-        <v>1538.770882119931</v>
+        <v>2088.3249137487501</v>
       </c>
       <c r="C32" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D32" s="2">
-        <v>4618.3848046873891</v>
+        <v>3746.5999999999972</v>
       </c>
       <c r="E32" s="2">
-        <v>55.071395338551852</v>
+        <v>44.99999999999995</v>
       </c>
       <c r="F32" s="2">
-        <v>114812.3437752546</v>
+        <v>84821.616612874292</v>
       </c>
       <c r="G32" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H32" s="2">
-        <v>38.340053815637972</v>
+        <v>54.072514242661697</v>
       </c>
       <c r="I32" s="2">
-        <v>12.28685519289307</v>
+        <v>9.9999999999999485</v>
       </c>
       <c r="J32" s="2">
-        <v>242.50619294031239</v>
+        <v>220.54621652251561</v>
       </c>
       <c r="K32" s="2">
-        <v>25539.762158507241</v>
+        <v>32749.978346102071</v>
       </c>
       <c r="L32" s="2">
-        <v>9173.571314907118</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M32" s="2">
-        <v>829678.14263907145</v>
+        <v>633508.48902710096</v>
       </c>
       <c r="N32" s="2">
-        <v>15.33792095756929</v>
+        <v>22.70687713300876</v>
       </c>
       <c r="O32" s="2">
-        <v>773.90834946545772</v>
+        <v>672.99999999999989</v>
       </c>
       <c r="P32" s="2">
-        <v>351134.24489040457</v>
+        <v>286032.99613732687</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -2024,28 +2024,28 @@
         <v>16685</v>
       </c>
       <c r="B33" s="2">
-        <v>3039.327255577944</v>
+        <v>2386</v>
       </c>
       <c r="C33" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D33" s="2">
-        <v>19721.961700869851</v>
+        <v>10592.2</v>
       </c>
       <c r="E33" s="2">
-        <v>462.59972084383571</v>
+        <v>377.99999999999972</v>
       </c>
       <c r="F33" s="2">
-        <v>576919.71193076542</v>
+        <v>398404.10684000002</v>
       </c>
       <c r="G33" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H33" s="2">
-        <v>32.530954752662552</v>
+        <v>54.072514242661697</v>
       </c>
       <c r="I33" s="2">
-        <v>28.259766943654089</v>
+        <v>28.221234650144272</v>
       </c>
       <c r="J33" s="2">
         <v>800.99999999999955</v>
@@ -2054,19 +2054,19 @@
         <v>112137</v>
       </c>
       <c r="L33" s="2">
-        <v>11325.753633906261</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M33" s="2">
-        <v>2178963.2517728689</v>
+        <v>1610842.1836000001</v>
       </c>
       <c r="N33" s="2">
-        <v>35.752251160859089</v>
+        <v>22.70687713300876</v>
       </c>
       <c r="O33" s="2">
-        <v>717.56138197094469</v>
+        <v>624.00000000000011</v>
       </c>
       <c r="P33" s="2">
-        <v>2250177.2411753312</v>
+        <v>1492496.0792400001</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -2077,7 +2077,7 @@
         <v>6906.9999999999973</v>
       </c>
       <c r="C34" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D34" s="2">
         <v>45679.399999999987</v>
@@ -2089,10 +2089,10 @@
         <v>1135992.2059200001</v>
       </c>
       <c r="G34" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H34" s="2">
-        <v>125.6772308691166</v>
+        <v>86.999999999999389</v>
       </c>
       <c r="I34" s="2">
         <v>196.9999999999992</v>
@@ -2101,22 +2101,22 @@
         <v>2450.9999999999991</v>
       </c>
       <c r="K34" s="2">
-        <v>54734.409810772122</v>
+        <v>49269.999999999927</v>
       </c>
       <c r="L34" s="2">
-        <v>12833.889841083959</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M34" s="2">
-        <v>1126650.8025755419</v>
+        <v>1321756.1130112109</v>
       </c>
       <c r="N34" s="2">
-        <v>35.752251160859089</v>
+        <v>26.99999999999994</v>
       </c>
       <c r="O34" s="2">
         <v>1960</v>
       </c>
       <c r="P34" s="2">
-        <v>2956763.3187957518</v>
+        <v>1961160.027659998</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -2124,49 +2124,49 @@
         <v>24184.999999999989</v>
       </c>
       <c r="B35" s="2">
-        <v>5648.5582401918809</v>
+        <v>4568.9999999999982</v>
       </c>
       <c r="C35" s="2">
         <v>21418.87329</v>
       </c>
       <c r="D35" s="2">
-        <v>6081.5841756274222</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E35" s="2">
-        <v>160.31895087445079</v>
+        <v>130.9999999999998</v>
       </c>
       <c r="F35" s="2">
-        <v>208070.17965088951</v>
+        <v>153719.09000888691</v>
       </c>
       <c r="G35" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H35" s="2">
-        <v>125.6772308691166</v>
+        <v>103.9999999999993</v>
       </c>
       <c r="I35" s="2">
-        <v>3.6860565578679099</v>
+        <v>2.999999999999976</v>
       </c>
       <c r="J35" s="2">
-        <v>361.93250076308379</v>
+        <v>479.14656225630722</v>
       </c>
       <c r="K35" s="2">
         <v>106498</v>
       </c>
       <c r="L35" s="2">
-        <v>23446.25551434037</v>
+        <v>19137.909999999989</v>
       </c>
       <c r="M35" s="2">
-        <v>4717355.206267274</v>
+        <v>3427876.6054999982</v>
       </c>
       <c r="N35" s="2">
         <v>50.999999999999893</v>
       </c>
       <c r="O35" s="2">
-        <v>1599.139320430128</v>
+        <v>1218</v>
       </c>
       <c r="P35" s="2">
-        <v>5013077.512856801</v>
+        <v>3524494.8488999992</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -2174,552 +2174,2803 @@
         <v>12565.999999999991</v>
       </c>
       <c r="B36" s="2">
-        <v>2667.372704601933</v>
+        <v>2093.9999999999991</v>
       </c>
       <c r="C36" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D36" s="2">
-        <v>8866.1006533160835</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E36" s="2">
-        <v>881.00766886934832</v>
+        <v>449.99999999999937</v>
       </c>
       <c r="F36" s="2">
-        <v>431856.96037441172</v>
+        <v>374829.37895564421</v>
       </c>
       <c r="G36" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H36" s="2">
-        <v>69.709188755705398</v>
+        <v>59.999999999999581</v>
       </c>
       <c r="I36" s="2">
-        <v>18.4302827893396</v>
+        <v>28.221234650144272</v>
       </c>
       <c r="J36" s="2">
-        <v>657.77532591485419</v>
+        <v>647.79999999999916</v>
       </c>
       <c r="K36" s="2">
-        <v>28572.53948311467</v>
+        <v>32749.978346102071</v>
       </c>
       <c r="L36" s="2">
-        <v>25487.601136104411</v>
+        <v>20804.14999999998</v>
       </c>
       <c r="M36" s="2">
-        <v>2074503.3200577251</v>
+        <v>1533618.0888999989</v>
       </c>
       <c r="N36" s="2">
-        <v>35.752251160859089</v>
+        <v>22.70687713300876</v>
       </c>
       <c r="O36" s="2">
-        <v>778.50810191398898</v>
+        <v>676.99999999999955</v>
       </c>
       <c r="P36" s="2">
-        <v>2817127.1114290119</v>
+        <v>1868542.2159599981</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>4183.9999999999918</v>
+        <v>17499</v>
       </c>
       <c r="B37" s="2">
-        <v>1005.041577808463</v>
+        <v>2815</v>
       </c>
       <c r="C37" s="2">
-        <v>20815.4167831292</v>
+        <v>20675.747319999999</v>
       </c>
       <c r="D37" s="2">
-        <v>2244.722876564279</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E37" s="2">
-        <v>97.904702824092013</v>
+        <v>387.99999999999977</v>
       </c>
       <c r="F37" s="2">
-        <v>83942.996320470527</v>
+        <v>509272.59584000002</v>
       </c>
       <c r="G37" s="2">
-        <v>35.799999999999997</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H37" s="2">
-        <v>15.103657563736149</v>
+        <v>54.072514242661697</v>
       </c>
       <c r="I37" s="2">
-        <v>2.4573710385786072</v>
+        <v>31.999999999999861</v>
       </c>
       <c r="J37" s="2">
-        <v>92.937872435693933</v>
+        <v>1231.9999999999991</v>
       </c>
       <c r="K37" s="2">
-        <v>35561.258219050636</v>
+        <v>47001.999999999993</v>
       </c>
       <c r="L37" s="2">
-        <v>1524.6140846819719</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M37" s="2">
-        <v>1134350.952355311</v>
+        <v>2998146.3123999988</v>
       </c>
       <c r="N37" s="2">
-        <v>10.225280638379511</v>
+        <v>22.70687713300876</v>
       </c>
       <c r="O37" s="2">
-        <v>289.78440425749631</v>
+        <v>1535</v>
       </c>
       <c r="P37" s="2">
-        <v>1130904.8238936481</v>
+        <v>4597855.1592400009</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>25263.999999999989</v>
+        <v>22832.999999999989</v>
       </c>
       <c r="B38" s="2">
-        <v>5648.5582401918809</v>
+        <v>2624.9999999999968</v>
       </c>
       <c r="C38" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D38" s="2">
-        <v>19721.961700869851</v>
+        <v>12773.499999999991</v>
       </c>
       <c r="E38" s="2">
-        <v>34.266645988432209</v>
+        <v>480.99999999999937</v>
       </c>
       <c r="F38" s="2">
-        <v>388747.33004037431</v>
+        <v>477102.61020999961</v>
       </c>
       <c r="G38" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H38" s="2">
-        <v>125.6772308691166</v>
+        <v>83.999999999999417</v>
       </c>
       <c r="I38" s="2">
-        <v>77.805859831260051</v>
+        <v>66.999999999999702</v>
       </c>
       <c r="J38" s="2">
-        <v>231.3171124750813</v>
+        <v>586.09999999999911</v>
       </c>
       <c r="K38" s="2">
-        <v>314708.99999999988</v>
+        <v>13303.99999999998</v>
       </c>
       <c r="L38" s="2">
-        <v>23252.7844053831</v>
+        <v>31991.309999999979</v>
       </c>
       <c r="M38" s="2">
-        <v>4717355.206267274</v>
+        <v>2339528.865499998</v>
       </c>
       <c r="N38" s="2">
-        <v>35.752251160859089</v>
+        <v>40.999999999999879</v>
       </c>
       <c r="O38" s="2">
-        <v>1599.139320430128</v>
+        <v>960.99999999999955</v>
       </c>
       <c r="P38" s="2">
-        <v>5013077.512856801</v>
+        <v>623372.23123661522</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>17569.999999999989</v>
+        <v>15277.999999999991</v>
       </c>
       <c r="B39" s="2">
-        <v>2404.9664117900902</v>
+        <v>2241.9999999999991</v>
       </c>
       <c r="C39" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D39" s="2">
-        <v>10460.827718341459</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E39" s="2">
-        <v>287.5950645457707</v>
+        <v>281.9402175474014</v>
       </c>
       <c r="F39" s="2">
-        <v>494652.20417661691</v>
+        <v>374829.37895564421</v>
       </c>
       <c r="G39" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H39" s="2">
-        <v>155.99999999999889</v>
+        <v>54.999999999999609</v>
       </c>
       <c r="I39" s="2">
-        <v>77.805859831260051</v>
+        <v>34.999999999999837</v>
       </c>
       <c r="J39" s="2">
-        <v>657.77532591485419</v>
+        <v>982.89999999999884</v>
       </c>
       <c r="K39" s="2">
-        <v>182951.9999999998</v>
+        <v>32749.978346102071</v>
       </c>
       <c r="L39" s="2">
-        <v>23401.03629808141</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M39" s="2">
-        <v>4717355.206267274</v>
+        <v>1321756.1130112109</v>
       </c>
       <c r="N39" s="2">
-        <v>35.752251160859089</v>
+        <v>24.999999999999929</v>
       </c>
       <c r="O39" s="2">
-        <v>909.60104669714224</v>
+        <v>693.99999999999932</v>
       </c>
       <c r="P39" s="2">
-        <v>486123.80006066471</v>
+        <v>3344506.7167999982</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>120926</v>
+        <v>9624.9999999999891</v>
       </c>
       <c r="B40" s="2">
-        <v>20038</v>
+        <v>2088.3249137487501</v>
       </c>
       <c r="C40" s="2">
-        <v>29031.0083701363</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D40" s="2">
-        <v>72911.599999999991</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E40" s="2">
-        <v>2549.9999999999982</v>
+        <v>135.9999999999998</v>
       </c>
       <c r="F40" s="2">
-        <v>4713511.9352799999</v>
+        <v>169429.59635735271</v>
       </c>
       <c r="G40" s="2">
-        <v>29.9</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H40" s="2">
-        <v>195.99999999999869</v>
+        <v>54.072514242661697</v>
       </c>
       <c r="I40" s="2">
-        <v>248.99999999999889</v>
+        <v>8.9999999999999467</v>
       </c>
       <c r="J40" s="2">
-        <v>1123.199999999998</v>
+        <v>175.79319424322901</v>
       </c>
       <c r="K40" s="2">
-        <v>1264806.9999999991</v>
+        <v>61603.99999999992</v>
       </c>
       <c r="L40" s="2">
-        <v>104307.93</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M40" s="2">
-        <v>2214641.3434399972</v>
+        <v>631359.22812760074</v>
       </c>
       <c r="N40" s="2">
-        <v>34.999999999999908</v>
+        <v>31.99999999999989</v>
       </c>
       <c r="O40" s="2">
-        <v>6308.9999999999991</v>
+        <v>609.58223327103974</v>
       </c>
       <c r="P40" s="2">
-        <v>26988496.705479991</v>
+        <v>105350.83313712729</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>50473.999999999993</v>
+        <v>7424.9999999999973</v>
       </c>
       <c r="B41" s="2">
-        <v>8680.9999999999982</v>
+        <v>2088.3249137487501</v>
       </c>
       <c r="C41" s="2">
-        <v>20815.4167831292</v>
+        <v>19210.228831246099</v>
       </c>
       <c r="D41" s="2">
-        <v>32935.899999999987</v>
+        <v>7762.6753209116032</v>
       </c>
       <c r="E41" s="2">
-        <v>1673.999999999998</v>
+        <v>119.9999999999999</v>
       </c>
       <c r="F41" s="2">
-        <v>1330729.4930400001</v>
+        <v>374829.37895564421</v>
       </c>
       <c r="G41" s="2">
-        <v>30.831632653061199</v>
+        <v>35.438037383177502</v>
       </c>
       <c r="H41" s="2">
-        <v>158.99999999999889</v>
+        <v>20.999999999999861</v>
       </c>
       <c r="I41" s="2">
-        <v>184.9999999999992</v>
+        <v>28.221234650144272</v>
       </c>
       <c r="J41" s="2">
-        <v>657.77532591485419</v>
+        <v>159.69871987364829</v>
       </c>
       <c r="K41" s="2">
-        <v>810919.99999999977</v>
+        <v>32749.978346102071</v>
       </c>
       <c r="L41" s="2">
-        <v>182696</v>
+        <v>14259.056285147481</v>
       </c>
       <c r="M41" s="2">
-        <v>5519372.8535999991</v>
+        <v>1321756.1130112109</v>
       </c>
       <c r="N41" s="2">
-        <v>38.999999999999908</v>
+        <v>22.70687713300876</v>
       </c>
       <c r="O41" s="2">
-        <v>2500</v>
+        <v>609.58223327103974</v>
       </c>
       <c r="P41" s="2">
-        <v>5013077.512856801</v>
+        <v>151489.05336028291</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>23671.999999999989</v>
+        <v>4183.9999999999918</v>
       </c>
       <c r="B42" s="2">
-        <v>3592.1638142203678</v>
+        <v>1056.473753859249</v>
       </c>
       <c r="C42" s="2">
-        <v>20815.4167831292</v>
+        <v>20427.341848341399</v>
       </c>
       <c r="D42" s="2">
-        <v>19721.961700869851</v>
+        <v>2381.065679515827</v>
       </c>
       <c r="E42" s="2">
-        <v>424.66164849949968</v>
+        <v>113.4249949517034</v>
       </c>
       <c r="F42" s="2">
-        <v>1094086.860592877</v>
+        <v>81501.246245260627</v>
       </c>
       <c r="G42" s="2">
-        <v>30.831632653061199</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="H42" s="2">
-        <v>125.6772308691166</v>
+        <v>15.982526713303701</v>
       </c>
       <c r="I42" s="2">
-        <v>77.805859831260051</v>
+        <v>2.5736340998794449</v>
       </c>
       <c r="J42" s="2">
-        <v>657.77532591485419</v>
+        <v>109.9937054332045</v>
       </c>
       <c r="K42" s="2">
-        <v>44036.371116277784</v>
+        <v>44335.913688073488</v>
       </c>
       <c r="L42" s="2">
-        <v>11411.26707998794</v>
+        <v>2003.2628205799081</v>
       </c>
       <c r="M42" s="2">
-        <v>4717355.206267274</v>
+        <v>1077875.2283725089</v>
       </c>
       <c r="N42" s="2">
-        <v>35.752251160859089</v>
+        <v>11.577914620948469</v>
       </c>
       <c r="O42" s="2">
-        <v>856.70389353902783</v>
+        <v>315.84662311287587</v>
       </c>
       <c r="P42" s="2">
-        <v>1248365.7581963211</v>
+        <v>1122077.8321941849</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>116468</v>
+        <v>25263.999999999989</v>
       </c>
       <c r="B43" s="2">
-        <v>21239</v>
+        <v>5714.5080545330657</v>
       </c>
       <c r="C43" s="2">
-        <v>29031.0083701363</v>
+        <v>20441.322639999999</v>
       </c>
       <c r="D43" s="2">
-        <v>64664.399999999987</v>
+        <v>18620.078602856651</v>
       </c>
       <c r="E43" s="2">
-        <v>2077</v>
+        <v>39.698748233096183</v>
       </c>
       <c r="F43" s="2">
-        <v>4676977.1911800001</v>
+        <v>377439.37268869882</v>
       </c>
       <c r="G43" s="2">
-        <v>30.2</v>
+        <v>28.859170731707302</v>
       </c>
       <c r="H43" s="2">
-        <v>300.99999999999812</v>
+        <v>121.2195445843775</v>
       </c>
       <c r="I43" s="2">
-        <v>303.99999999999869</v>
+        <v>82.574144705994001</v>
       </c>
       <c r="J43" s="2">
-        <v>783.79999999999882</v>
+        <v>273.76811696274279</v>
       </c>
       <c r="K43" s="2">
-        <v>202571</v>
+        <v>390629.37411319528</v>
       </c>
       <c r="L43" s="2">
-        <v>87368.909999999974</v>
+        <v>30552.937259516999</v>
       </c>
       <c r="M43" s="2">
-        <v>8408723.8795999978</v>
+        <v>5170690.3577637998</v>
       </c>
       <c r="N43" s="2">
-        <v>34.999999999999901</v>
+        <v>37.037791832750607</v>
       </c>
       <c r="O43" s="2">
-        <v>4502</v>
+        <v>1578.0387530220919</v>
       </c>
       <c r="P43" s="2">
-        <v>25333054.934995431</v>
+        <v>5162046.5029202029</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>64841.999999999993</v>
+        <v>17569.999999999989</v>
       </c>
       <c r="B44" s="2">
-        <v>15029</v>
+        <v>2528.0385897164319</v>
       </c>
       <c r="C44" s="2">
-        <v>25869.387780000001</v>
+        <v>20427.341848341399</v>
       </c>
       <c r="D44" s="2">
-        <v>19151.026043098391</v>
+        <v>11096.210636742029</v>
       </c>
       <c r="E44" s="2">
-        <v>1645.6410443006489</v>
+        <v>333.18592267062911</v>
       </c>
       <c r="F44" s="2">
-        <v>1067319.0716998819</v>
+        <v>480263.66540990549</v>
       </c>
       <c r="G44" s="2">
-        <v>27.620294559099399</v>
+        <v>28.859170731707302</v>
       </c>
       <c r="H44" s="2">
-        <v>124.9999999999992</v>
+        <v>155.99999999999889</v>
       </c>
       <c r="I44" s="2">
-        <v>194.99999999999909</v>
+        <v>82.574144705994001</v>
       </c>
       <c r="J44" s="2">
-        <v>384.78892776104192</v>
+        <v>675.1104937785783</v>
       </c>
       <c r="K44" s="2">
-        <v>2168.999999999995</v>
+        <v>253392.3988960179</v>
       </c>
       <c r="L44" s="2">
-        <v>24766.251315762191</v>
+        <v>30747.732458975679</v>
       </c>
       <c r="M44" s="2">
-        <v>282905.75142886041</v>
+        <v>3041350.614883801</v>
       </c>
       <c r="N44" s="2">
-        <v>21.095615783084529</v>
+        <v>37.037791832750607</v>
       </c>
       <c r="O44" s="2">
-        <v>3211</v>
+        <v>1578.0387530220919</v>
       </c>
       <c r="P44" s="2">
-        <v>9430951.7147999946</v>
+        <v>482329.48363598721</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>64100</v>
+        <v>120926</v>
       </c>
       <c r="B45" s="2">
-        <v>9192</v>
+        <v>20038</v>
       </c>
       <c r="C45" s="2">
-        <v>21205.026720000002</v>
+        <v>25152.816680000011</v>
       </c>
       <c r="D45" s="2">
-        <v>59994</v>
+        <v>72911.599999999991</v>
       </c>
       <c r="E45" s="2">
-        <v>1042.9999999999991</v>
+        <v>2549.9999999999982</v>
       </c>
       <c r="F45" s="2">
-        <v>1194600.348719999</v>
+        <v>4713511.9352799999</v>
       </c>
       <c r="G45" s="2">
-        <v>30.831632653061199</v>
+        <v>29.9</v>
       </c>
       <c r="H45" s="2">
-        <v>140.99999999999909</v>
+        <v>195.99999999999869</v>
       </c>
       <c r="I45" s="2">
-        <v>92.999999999999559</v>
+        <v>248.99999999999889</v>
       </c>
       <c r="J45" s="2">
-        <v>657.77532591485419</v>
+        <v>1123.199999999998</v>
       </c>
       <c r="K45" s="2">
-        <v>39877.133642530513</v>
+        <v>1264806.9999999991</v>
       </c>
       <c r="L45" s="2">
-        <v>70633.640917482451</v>
+        <v>104307.93</v>
       </c>
       <c r="M45" s="2">
-        <v>8271274.1760000018</v>
+        <v>2846566.7104680962</v>
       </c>
       <c r="N45" s="2">
-        <v>36.999999999999908</v>
+        <v>37.037791832750607</v>
       </c>
       <c r="O45" s="2">
-        <v>3090</v>
+        <v>6308.9999999999991</v>
       </c>
       <c r="P45" s="2">
-        <v>7029925.2345599988</v>
+        <v>26988496.705479991</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
+        <v>50473.999999999993</v>
+      </c>
+      <c r="B46" s="2">
+        <v>8680.9999999999982</v>
+      </c>
+      <c r="C46" s="2">
+        <v>20427.341848341399</v>
+      </c>
+      <c r="D46" s="2">
+        <v>32935.899999999987</v>
+      </c>
+      <c r="E46" s="2">
+        <v>1673.999999999998</v>
+      </c>
+      <c r="F46" s="2">
+        <v>1330729.4930400001</v>
+      </c>
+      <c r="G46" s="2">
+        <v>28.859170731707302</v>
+      </c>
+      <c r="H46" s="2">
+        <v>158.99999999999889</v>
+      </c>
+      <c r="I46" s="2">
+        <v>184.9999999999992</v>
+      </c>
+      <c r="J46" s="2">
+        <v>675.1104937785783</v>
+      </c>
+      <c r="K46" s="2">
+        <v>810919.99999999977</v>
+      </c>
+      <c r="L46" s="2">
+        <v>182696</v>
+      </c>
+      <c r="M46" s="2">
+        <v>5519372.8535999991</v>
+      </c>
+      <c r="N46" s="2">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="O46" s="2">
+        <v>2500</v>
+      </c>
+      <c r="P46" s="2">
+        <v>5162046.5029202029</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>8854.9999999999945</v>
+      </c>
+      <c r="B47" s="2">
+        <v>1712.585464114045</v>
+      </c>
+      <c r="C47" s="2">
+        <v>2742.4423706999132</v>
+      </c>
+      <c r="D47" s="2">
+        <v>368.73175267625697</v>
+      </c>
+      <c r="E47" s="2">
+        <v>415783.74875999981</v>
+      </c>
+      <c r="F47" s="2">
+        <v>66.01616609003284</v>
+      </c>
+      <c r="G47" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H47" s="2">
+        <v>20.900227240474099</v>
+      </c>
+      <c r="I47" s="2">
+        <v>20.58907279903562</v>
+      </c>
+      <c r="J47" s="2">
+        <v>675.1104937785783</v>
+      </c>
+      <c r="K47" s="2">
+        <v>123470.76207345699</v>
+      </c>
+      <c r="L47" s="2">
+        <v>12349.96091436373</v>
+      </c>
+      <c r="M47" s="2">
+        <v>5170690.3577637998</v>
+      </c>
+      <c r="N47" s="2">
+        <v>37.037791832750607</v>
+      </c>
+      <c r="O47" s="2">
+        <v>472.51657505378728</v>
+      </c>
+      <c r="P47" s="2">
+        <v>547666.4329575079</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>17833.999999999989</v>
+      </c>
+      <c r="B48" s="2">
+        <v>2794.5002842892968</v>
+      </c>
+      <c r="C48" s="2">
+        <v>6823.8075820629474</v>
+      </c>
+      <c r="D48" s="2">
+        <v>275.89503480386611</v>
+      </c>
+      <c r="E48" s="2">
+        <v>267414.72804000002</v>
+      </c>
+      <c r="F48" s="2">
+        <v>21.08181093591994</v>
+      </c>
+      <c r="G48" s="2">
+        <v>32.08</v>
+      </c>
+      <c r="H48" s="2">
+        <v>121.2195445843775</v>
+      </c>
+      <c r="I48" s="2">
+        <v>82.574144705994001</v>
+      </c>
+      <c r="J48" s="2">
+        <v>675.1104937785783</v>
+      </c>
+      <c r="K48" s="2">
+        <v>390629.37411319528</v>
+      </c>
+      <c r="L48" s="2">
+        <v>27310.927642478491</v>
+      </c>
+      <c r="M48" s="2">
+        <v>3230208.689405594</v>
+      </c>
+      <c r="N48" s="2">
+        <v>39.999999999999893</v>
+      </c>
+      <c r="O48" s="2">
+        <v>1578.0387530220919</v>
+      </c>
+      <c r="P48" s="2">
+        <v>2346273.839680803</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>22243.999999999989</v>
+      </c>
+      <c r="B49" s="2">
+        <v>3600.5803854594751</v>
+      </c>
+      <c r="C49" s="2">
+        <v>9562.6435694480715</v>
+      </c>
+      <c r="D49" s="2">
+        <v>268.04967836394559</v>
+      </c>
+      <c r="E49" s="2">
+        <v>229243.99999999991</v>
+      </c>
+      <c r="F49" s="2">
+        <v>14.489601624263949</v>
+      </c>
+      <c r="G49" s="2">
+        <v>28.859170731707302</v>
+      </c>
+      <c r="H49" s="2">
+        <v>121.2195445843775</v>
+      </c>
+      <c r="I49" s="2">
+        <v>39.891328548131497</v>
+      </c>
+      <c r="J49" s="2">
+        <v>133.23561862056471</v>
+      </c>
+      <c r="K49" s="2">
+        <v>390629.37411319528</v>
+      </c>
+      <c r="L49" s="2">
+        <v>7929.602119936877</v>
+      </c>
+      <c r="M49" s="2">
+        <v>5170690.3577637998</v>
+      </c>
+      <c r="N49" s="2">
+        <v>37.037791832750607</v>
+      </c>
+      <c r="O49" s="2">
+        <v>1578.0387530220919</v>
+      </c>
+      <c r="P49" s="2">
+        <v>900544.63312254427</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>35142.999999999993</v>
+      </c>
+      <c r="B50" s="2">
+        <v>5714.5080545330657</v>
+      </c>
+      <c r="C50" s="2">
+        <v>27639.69999999999</v>
+      </c>
+      <c r="D50" s="2">
+        <v>287.66306946374652</v>
+      </c>
+      <c r="E50" s="2">
+        <v>794230.03655999957</v>
+      </c>
+      <c r="F50" s="2">
+        <v>31.774507571663939</v>
+      </c>
+      <c r="G50" s="2">
+        <v>28.859170731707302</v>
+      </c>
+      <c r="H50" s="2">
+        <v>125.9999999999992</v>
+      </c>
+      <c r="I50" s="2">
+        <v>95.999999999999559</v>
+      </c>
+      <c r="J50" s="2">
+        <v>675.1104937785783</v>
+      </c>
+      <c r="K50" s="2">
+        <v>390629.37411319528</v>
+      </c>
+      <c r="L50" s="2">
+        <v>14603.603416984841</v>
+      </c>
+      <c r="M50" s="2">
+        <v>8906174.1647999976</v>
+      </c>
+      <c r="N50" s="2">
+        <v>37.037791832750607</v>
+      </c>
+      <c r="O50" s="2">
+        <v>1578.0387530220919</v>
+      </c>
+      <c r="P50" s="2">
+        <v>5162046.5029202029</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>31885.999999999989</v>
+      </c>
+      <c r="B51" s="2">
+        <v>5714.5080545330657</v>
+      </c>
+      <c r="C51" s="2">
+        <v>10600.43340332655</v>
+      </c>
+      <c r="D51" s="2">
+        <v>457.64579232868749</v>
+      </c>
+      <c r="E51" s="2">
+        <v>135007.86686999991</v>
+      </c>
+      <c r="F51" s="2">
+        <v>5.9529246791480057</v>
+      </c>
+      <c r="G51" s="2">
+        <v>28.859170731707302</v>
+      </c>
+      <c r="H51" s="2">
+        <v>126.9999999999992</v>
+      </c>
+      <c r="I51" s="2">
+        <v>32.170426248493158</v>
+      </c>
+      <c r="J51" s="2">
+        <v>675.1104937785783</v>
+      </c>
+      <c r="K51" s="2">
+        <v>532404</v>
+      </c>
+      <c r="L51" s="2">
+        <v>50169.914191199998</v>
+      </c>
+      <c r="M51" s="2">
+        <v>9174521.0092999972</v>
+      </c>
+      <c r="N51" s="2">
+        <v>37.037791832750607</v>
+      </c>
+      <c r="O51" s="2">
+        <v>2097</v>
+      </c>
+      <c r="P51" s="2">
+        <v>17566777.100189991</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>23671.999999999989</v>
+      </c>
+      <c r="B52" s="2">
+        <v>5316.1026797151171</v>
+      </c>
+      <c r="C52" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D52" s="2">
+        <v>18102.33886557139</v>
+      </c>
+      <c r="E52" s="2">
+        <v>692.21862862467367</v>
+      </c>
+      <c r="F52" s="2">
+        <v>786293.0504705467</v>
+      </c>
+      <c r="G52" s="2">
+        <v>28</v>
+      </c>
+      <c r="H52" s="2">
+        <v>90.463582676213051</v>
+      </c>
+      <c r="I52" s="2">
+        <v>70.480699544079414</v>
+      </c>
+      <c r="J52" s="2">
+        <v>497.85288158683818</v>
+      </c>
+      <c r="K52" s="2">
+        <v>61373.672326328422</v>
+      </c>
+      <c r="L52" s="2">
+        <v>12579.47779916077</v>
+      </c>
+      <c r="M52" s="2">
+        <v>3234408.7671999992</v>
+      </c>
+      <c r="N52" s="2">
+        <v>28.514194264827129</v>
+      </c>
+      <c r="O52" s="2">
+        <v>801.10415672385136</v>
+      </c>
+      <c r="P52" s="2">
+        <v>1155335.2855618461</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>116468</v>
+      </c>
+      <c r="B53" s="2">
+        <v>21239</v>
+      </c>
+      <c r="C53" s="2">
+        <v>23604.910929999998</v>
+      </c>
+      <c r="D53" s="2">
+        <v>64664.399999999987</v>
+      </c>
+      <c r="E53" s="2">
+        <v>2077</v>
+      </c>
+      <c r="F53" s="2">
+        <v>4676977.1911800001</v>
+      </c>
+      <c r="G53" s="2">
+        <v>30.2</v>
+      </c>
+      <c r="H53" s="2">
+        <v>300.99999999999812</v>
+      </c>
+      <c r="I53" s="2">
+        <v>303.99999999999869</v>
+      </c>
+      <c r="J53" s="2">
+        <v>783.79999999999882</v>
+      </c>
+      <c r="K53" s="2">
+        <v>202571</v>
+      </c>
+      <c r="L53" s="2">
+        <v>87368.909999999974</v>
+      </c>
+      <c r="M53" s="2">
+        <v>8408723.8795999978</v>
+      </c>
+      <c r="N53" s="2">
+        <v>34.999999999999901</v>
+      </c>
+      <c r="O53" s="2">
+        <v>4502</v>
+      </c>
+      <c r="P53" s="2">
+        <v>19397519.885310002</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>64841.999999999993</v>
+      </c>
+      <c r="B54" s="2">
+        <v>15029</v>
+      </c>
+      <c r="C54" s="2">
+        <v>25869.387780000001</v>
+      </c>
+      <c r="D54" s="2">
+        <v>18102.33886557139</v>
+      </c>
+      <c r="E54" s="2">
+        <v>1123.9999999999991</v>
+      </c>
+      <c r="F54" s="2">
+        <v>866008.93850999954</v>
+      </c>
+      <c r="G54" s="2">
+        <v>26.112401315789398</v>
+      </c>
+      <c r="H54" s="2">
+        <v>124.9999999999992</v>
+      </c>
+      <c r="I54" s="2">
+        <v>194.99999999999909</v>
+      </c>
+      <c r="J54" s="2">
+        <v>257.87557539933027</v>
+      </c>
+      <c r="K54" s="2">
+        <v>2327.949027416018</v>
+      </c>
+      <c r="L54" s="2">
+        <v>29602.9087374105</v>
+      </c>
+      <c r="M54" s="2">
+        <v>352889.09448255628</v>
+      </c>
+      <c r="N54" s="2">
+        <v>11.99999999999995</v>
+      </c>
+      <c r="O54" s="2">
+        <v>3211</v>
+      </c>
+      <c r="P54" s="2">
+        <v>9430951.7147999946</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>64100</v>
+      </c>
+      <c r="B55" s="2">
+        <v>9192</v>
+      </c>
+      <c r="C55" s="2">
+        <v>21205.026720000002</v>
+      </c>
+      <c r="D55" s="2">
+        <v>59994</v>
+      </c>
+      <c r="E55" s="2">
+        <v>1042.9999999999991</v>
+      </c>
+      <c r="F55" s="2">
+        <v>1194600.348719999</v>
+      </c>
+      <c r="G55" s="2">
+        <v>26.112401315789398</v>
+      </c>
+      <c r="H55" s="2">
+        <v>140.99999999999909</v>
+      </c>
+      <c r="I55" s="2">
+        <v>92.999999999999559</v>
+      </c>
+      <c r="J55" s="2">
+        <v>563.59999999999923</v>
+      </c>
+      <c r="K55" s="2">
+        <v>61373.672326328422</v>
+      </c>
+      <c r="L55" s="2">
+        <v>57654.419999999991</v>
+      </c>
+      <c r="M55" s="2">
+        <v>8271274.1760000018</v>
+      </c>
+      <c r="N55" s="2">
+        <v>36.999999999999908</v>
+      </c>
+      <c r="O55" s="2">
+        <v>3090</v>
+      </c>
+      <c r="P55" s="2">
+        <v>7029925.2345599988</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
         <v>105038</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B56" s="2">
         <v>11442</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C56" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D56" s="2">
+        <v>69421.599999999991</v>
+      </c>
+      <c r="E56" s="2">
+        <v>104.0508328856842</v>
+      </c>
+      <c r="F56" s="2">
+        <v>3389505.0556999999</v>
+      </c>
+      <c r="G56" s="2">
+        <v>26.112401315789398</v>
+      </c>
+      <c r="H56" s="2">
+        <v>164.99999999999889</v>
+      </c>
+      <c r="I56" s="2">
+        <v>248.99999999999901</v>
+      </c>
+      <c r="J56" s="2">
+        <v>497.85288158683818</v>
+      </c>
+      <c r="K56" s="2">
+        <v>19594.912583464229</v>
+      </c>
+      <c r="L56" s="2">
+        <v>57789.999999999949</v>
+      </c>
+      <c r="M56" s="2">
+        <v>708166.29511669534</v>
+      </c>
+      <c r="N56" s="2">
+        <v>5.9999999999999627</v>
+      </c>
+      <c r="O56" s="2">
+        <v>3403</v>
+      </c>
+      <c r="P56" s="2">
+        <v>5939939.1027600002</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>22677.999999999989</v>
+      </c>
+      <c r="B57" s="2">
+        <v>2850.946154295078</v>
+      </c>
+      <c r="C57" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D57" s="2">
+        <v>18102.33886557139</v>
+      </c>
+      <c r="E57" s="2">
+        <v>692.21862862467367</v>
+      </c>
+      <c r="F57" s="2">
+        <v>786293.0504705467</v>
+      </c>
+      <c r="G57" s="2">
+        <v>26.112401315789398</v>
+      </c>
+      <c r="H57" s="2">
+        <v>90.463582676213051</v>
+      </c>
+      <c r="I57" s="2">
+        <v>38.934050597635931</v>
+      </c>
+      <c r="J57" s="2">
+        <v>497.85288158683818</v>
+      </c>
+      <c r="K57" s="2">
+        <v>15515.367054092199</v>
+      </c>
+      <c r="L57" s="2">
+        <v>35901.050000000003</v>
+      </c>
+      <c r="M57" s="2">
+        <v>2185490.0203954638</v>
+      </c>
+      <c r="N57" s="2">
+        <v>28.514194264827129</v>
+      </c>
+      <c r="O57" s="2">
+        <v>1635.6427628317319</v>
+      </c>
+      <c r="P57" s="2">
+        <v>1301161.1051647051</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>17174.999999999989</v>
+      </c>
+      <c r="B58" s="2">
+        <v>2608.1457950007161</v>
+      </c>
+      <c r="C58" s="2">
+        <v>22823.19152</v>
+      </c>
+      <c r="D58" s="2">
+        <v>7865.8328546353896</v>
+      </c>
+      <c r="E58" s="2">
+        <v>318.65567571240911</v>
+      </c>
+      <c r="F58" s="2">
+        <v>310464.05231932248</v>
+      </c>
+      <c r="G58" s="2">
+        <v>27.3</v>
+      </c>
+      <c r="H58" s="2">
+        <v>90.463582676213051</v>
+      </c>
+      <c r="I58" s="2">
+        <v>9.4385577206390021</v>
+      </c>
+      <c r="J58" s="2">
+        <v>89.062380118800007</v>
+      </c>
+      <c r="K58" s="2">
+        <v>86576.999999999913</v>
+      </c>
+      <c r="L58" s="2">
+        <v>29602.9087374105</v>
+      </c>
+      <c r="M58" s="2">
+        <v>2185490.0203954638</v>
+      </c>
+      <c r="N58" s="2">
+        <v>28.514194264827129</v>
+      </c>
+      <c r="O58" s="2">
+        <v>784.97454283008244</v>
+      </c>
+      <c r="P58" s="2">
+        <v>2038235.528024235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>39066.999999999993</v>
+      </c>
+      <c r="B59" s="2">
+        <v>6011.9999999999982</v>
+      </c>
+      <c r="C59" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D59" s="2">
+        <v>20455.999999999989</v>
+      </c>
+      <c r="E59" s="2">
+        <v>692.21862862467367</v>
+      </c>
+      <c r="F59" s="2">
+        <v>899043.39099999995</v>
+      </c>
+      <c r="G59" s="2">
+        <v>37.19</v>
+      </c>
+      <c r="H59" s="2">
+        <v>147.99999999999909</v>
+      </c>
+      <c r="I59" s="2">
+        <v>70.480699544079414</v>
+      </c>
+      <c r="J59" s="2">
+        <v>618.49999999999932</v>
+      </c>
+      <c r="K59" s="2">
+        <v>29004.37737062724</v>
+      </c>
+      <c r="L59" s="2">
+        <v>29602.9087374105</v>
+      </c>
+      <c r="M59" s="2">
+        <v>2652645.5177999991</v>
+      </c>
+      <c r="N59" s="2">
+        <v>28.514194264827129</v>
+      </c>
+      <c r="O59" s="2">
+        <v>1635.6427628317319</v>
+      </c>
+      <c r="P59" s="2">
+        <v>6067714.9468499981</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>27626.999999999989</v>
+      </c>
+      <c r="B60" s="2">
+        <v>5316.1026797151171</v>
+      </c>
+      <c r="C60" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D60" s="2">
+        <v>18102.33886557139</v>
+      </c>
+      <c r="E60" s="2">
+        <v>1097.9999999999991</v>
+      </c>
+      <c r="F60" s="2">
+        <v>786293.0504705467</v>
+      </c>
+      <c r="G60" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="H60" s="2">
+        <v>122.9999999999992</v>
+      </c>
+      <c r="I60" s="2">
+        <v>70.480699544079414</v>
+      </c>
+      <c r="J60" s="2">
+        <v>497.85288158683818</v>
+      </c>
+      <c r="K60" s="2">
+        <v>61373.672326328422</v>
+      </c>
+      <c r="L60" s="2">
+        <v>29602.9087374105</v>
+      </c>
+      <c r="M60" s="2">
+        <v>2725337.6207999978</v>
+      </c>
+      <c r="N60" s="2">
+        <v>28.514194264827129</v>
+      </c>
+      <c r="O60" s="2">
+        <v>1635.6427628317319</v>
+      </c>
+      <c r="P60" s="2">
+        <v>776217.68512479798</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>31271</v>
+      </c>
+      <c r="B61" s="2">
+        <v>5316.1026797151171</v>
+      </c>
+      <c r="C61" s="2">
+        <v>20804.770158470299</v>
+      </c>
+      <c r="D61" s="2">
+        <v>18102.33886557139</v>
+      </c>
+      <c r="E61" s="2">
+        <v>692.21862862467367</v>
+      </c>
+      <c r="F61" s="2">
+        <v>411275.63845010422</v>
+      </c>
+      <c r="G61" s="2">
+        <v>29.58</v>
+      </c>
+      <c r="H61" s="2">
+        <v>90.463582676213051</v>
+      </c>
+      <c r="I61" s="2">
+        <v>113.9999999999995</v>
+      </c>
+      <c r="J61" s="2">
+        <v>497.85288158683818</v>
+      </c>
+      <c r="K61" s="2">
+        <v>116218</v>
+      </c>
+      <c r="L61" s="2">
+        <v>29804.749999999989</v>
+      </c>
+      <c r="M61" s="2">
+        <v>5228156.3358999994</v>
+      </c>
+      <c r="N61" s="2">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="O61" s="2">
+        <v>1635.6427628317319</v>
+      </c>
+      <c r="P61" s="2">
+        <v>3002048.203665785</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>9622.9999999999964</v>
+      </c>
+      <c r="B62" s="2">
+        <v>1538.770882119931</v>
+      </c>
+      <c r="C62" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D62" s="2">
+        <v>4618.3848046873891</v>
+      </c>
+      <c r="E62" s="2">
+        <v>55.071395338551852</v>
+      </c>
+      <c r="F62" s="2">
+        <v>114812.3437752546</v>
+      </c>
+      <c r="G62" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H62" s="2">
+        <v>38.340053815637972</v>
+      </c>
+      <c r="I62" s="2">
+        <v>12.28685519289307</v>
+      </c>
+      <c r="J62" s="2">
+        <v>242.50619294031239</v>
+      </c>
+      <c r="K62" s="2">
+        <v>25539.762158507241</v>
+      </c>
+      <c r="L62" s="2">
+        <v>9173.571314907118</v>
+      </c>
+      <c r="M62" s="2">
+        <v>829678.14263907145</v>
+      </c>
+      <c r="N62" s="2">
+        <v>15.33792095756929</v>
+      </c>
+      <c r="O62" s="2">
+        <v>773.90834946545772</v>
+      </c>
+      <c r="P62" s="2">
+        <v>351134.24489040457</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>16685</v>
+      </c>
+      <c r="B63" s="2">
+        <v>3039.327255577944</v>
+      </c>
+      <c r="C63" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D63" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E63" s="2">
+        <v>462.59972084383571</v>
+      </c>
+      <c r="F63" s="2">
+        <v>576919.71193076542</v>
+      </c>
+      <c r="G63" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H63" s="2">
+        <v>32.530954752662552</v>
+      </c>
+      <c r="I63" s="2">
+        <v>28.259766943654089</v>
+      </c>
+      <c r="J63" s="2">
+        <v>800.99999999999955</v>
+      </c>
+      <c r="K63" s="2">
+        <v>112137</v>
+      </c>
+      <c r="L63" s="2">
+        <v>11325.753633906261</v>
+      </c>
+      <c r="M63" s="2">
+        <v>2178963.2517728689</v>
+      </c>
+      <c r="N63" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O63" s="2">
+        <v>717.56138197094469</v>
+      </c>
+      <c r="P63" s="2">
+        <v>2250177.2411753312</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>40956</v>
+      </c>
+      <c r="B64" s="2">
+        <v>6906.9999999999973</v>
+      </c>
+      <c r="C64" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D64" s="2">
+        <v>45679.399999999987</v>
+      </c>
+      <c r="E64" s="2">
+        <v>943.99999999999955</v>
+      </c>
+      <c r="F64" s="2">
+        <v>1135992.2059200001</v>
+      </c>
+      <c r="G64" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H64" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I64" s="2">
+        <v>196.9999999999992</v>
+      </c>
+      <c r="J64" s="2">
+        <v>2450.9999999999991</v>
+      </c>
+      <c r="K64" s="2">
+        <v>54734.409810772122</v>
+      </c>
+      <c r="L64" s="2">
+        <v>12833.889841083959</v>
+      </c>
+      <c r="M64" s="2">
+        <v>1126650.8025755419</v>
+      </c>
+      <c r="N64" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O64" s="2">
+        <v>1960</v>
+      </c>
+      <c r="P64" s="2">
+        <v>2956763.3187957518</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>24184.999999999989</v>
+      </c>
+      <c r="B65" s="2">
+        <v>5648.5582401918809</v>
+      </c>
+      <c r="C65" s="2">
+        <v>21418.87329</v>
+      </c>
+      <c r="D65" s="2">
+        <v>6081.5841756274222</v>
+      </c>
+      <c r="E65" s="2">
+        <v>160.31895087445079</v>
+      </c>
+      <c r="F65" s="2">
+        <v>208070.17965088951</v>
+      </c>
+      <c r="G65" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H65" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I65" s="2">
+        <v>3.6860565578679099</v>
+      </c>
+      <c r="J65" s="2">
+        <v>361.93250076308379</v>
+      </c>
+      <c r="K65" s="2">
+        <v>106498</v>
+      </c>
+      <c r="L65" s="2">
+        <v>23446.25551434037</v>
+      </c>
+      <c r="M65" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N65" s="2">
+        <v>50.999999999999893</v>
+      </c>
+      <c r="O65" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P65" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>12565.999999999991</v>
+      </c>
+      <c r="B66" s="2">
+        <v>2667.372704601933</v>
+      </c>
+      <c r="C66" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D66" s="2">
+        <v>8866.1006533160835</v>
+      </c>
+      <c r="E66" s="2">
+        <v>881.00766886934832</v>
+      </c>
+      <c r="F66" s="2">
+        <v>431856.96037441172</v>
+      </c>
+      <c r="G66" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H66" s="2">
+        <v>69.709188755705398</v>
+      </c>
+      <c r="I66" s="2">
+        <v>18.4302827893396</v>
+      </c>
+      <c r="J66" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K66" s="2">
+        <v>28572.53948311467</v>
+      </c>
+      <c r="L66" s="2">
+        <v>25487.601136104411</v>
+      </c>
+      <c r="M66" s="2">
+        <v>2074503.3200577251</v>
+      </c>
+      <c r="N66" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O66" s="2">
+        <v>778.50810191398898</v>
+      </c>
+      <c r="P66" s="2">
+        <v>2817127.1114290119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>17499</v>
+      </c>
+      <c r="B67" s="2">
+        <v>3585.7947294433829</v>
+      </c>
+      <c r="C67" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D67" s="2">
+        <v>4985.6022373773949</v>
+      </c>
+      <c r="E67" s="2">
+        <v>474.83780869684728</v>
+      </c>
+      <c r="F67" s="2">
+        <v>737465.78973956313</v>
+      </c>
+      <c r="G67" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H67" s="2">
+        <v>62.738269880134887</v>
+      </c>
+      <c r="I67" s="2">
+        <v>39.31793661725785</v>
+      </c>
+      <c r="J67" s="2">
+        <v>1231.9999999999991</v>
+      </c>
+      <c r="K67" s="2">
+        <v>52214.87172571371</v>
+      </c>
+      <c r="L67" s="2">
+        <v>10989.33540619813</v>
+      </c>
+      <c r="M67" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N67" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O67" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P67" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>22832.999999999989</v>
+      </c>
+      <c r="B68" s="2">
+        <v>3343.7695079178939</v>
+      </c>
+      <c r="C68" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D68" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E68" s="2">
+        <v>881.00766886934832</v>
+      </c>
+      <c r="F68" s="2">
+        <v>690881.18249320716</v>
+      </c>
+      <c r="G68" s="2">
+        <v>32.450000000000003</v>
+      </c>
+      <c r="H68" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I68" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J68" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K68" s="2">
+        <v>14779.51264709787</v>
+      </c>
+      <c r="L68" s="2">
+        <v>39193.225827609822</v>
+      </c>
+      <c r="M68" s="2">
+        <v>3164647.3355904031</v>
+      </c>
+      <c r="N68" s="2">
+        <v>40.999999999999879</v>
+      </c>
+      <c r="O68" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P68" s="2">
+        <v>765252.05363309174</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>15277.999999999991</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2855.8976140007321</v>
+      </c>
+      <c r="C69" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D69" s="2">
+        <v>6933.370835542808</v>
+      </c>
+      <c r="E69" s="2">
+        <v>310.84743146649271</v>
+      </c>
+      <c r="F69" s="2">
+        <v>442174.81248465623</v>
+      </c>
+      <c r="G69" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H69" s="2">
+        <v>63.900089692729942</v>
+      </c>
+      <c r="I69" s="2">
+        <v>43.00399317512575</v>
+      </c>
+      <c r="J69" s="2">
+        <v>982.89999999999884</v>
+      </c>
+      <c r="K69" s="2">
+        <v>25352.018800317259</v>
+      </c>
+      <c r="L69" s="2">
+        <v>16214.47648840938</v>
+      </c>
+      <c r="M69" s="2">
+        <v>1683505.391251907</v>
+      </c>
+      <c r="N69" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O69" s="2">
+        <v>798.05704982024849</v>
+      </c>
+      <c r="P69" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>9624.9999999999891</v>
+      </c>
+      <c r="B70" s="2">
+        <v>1599.914095979</v>
+      </c>
+      <c r="C70" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D70" s="2">
+        <v>7805.2502922116228</v>
+      </c>
+      <c r="E70" s="2">
+        <v>166.4379948009566</v>
+      </c>
+      <c r="F70" s="2">
+        <v>229335.514217616</v>
+      </c>
+      <c r="G70" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H70" s="2">
+        <v>53.443711379374108</v>
+      </c>
+      <c r="I70" s="2">
+        <v>11.05816967360375</v>
+      </c>
+      <c r="J70" s="2">
+        <v>193.2970737513881</v>
+      </c>
+      <c r="K70" s="2">
+        <v>101102.97564972581</v>
+      </c>
+      <c r="L70" s="2">
+        <v>16989.97808396383</v>
+      </c>
+      <c r="M70" s="2">
+        <v>826863.3503797244</v>
+      </c>
+      <c r="N70" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O70" s="2">
+        <v>466.87487352596639</v>
+      </c>
+      <c r="P70" s="2">
+        <v>129328.7338934138</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>7424.9999999999973</v>
+      </c>
+      <c r="B71" s="2">
+        <v>1647.045323328701</v>
+      </c>
+      <c r="C71" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D71" s="2">
+        <v>5679.851509250544</v>
+      </c>
+      <c r="E71" s="2">
+        <v>146.85705423613831</v>
+      </c>
+      <c r="F71" s="2">
+        <v>317997.24106579472</v>
+      </c>
+      <c r="G71" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H71" s="2">
+        <v>24.398216064496889</v>
+      </c>
+      <c r="I71" s="2">
+        <v>22.116339347207528</v>
+      </c>
+      <c r="J71" s="2">
+        <v>175.60005872984959</v>
+      </c>
+      <c r="K71" s="2">
+        <v>18464.392641868159</v>
+      </c>
+      <c r="L71" s="2">
+        <v>14618.511356452391</v>
+      </c>
+      <c r="M71" s="2">
+        <v>1004420.350031578</v>
+      </c>
+      <c r="N71" s="2">
+        <v>15.33792095756929</v>
+      </c>
+      <c r="O71" s="2">
+        <v>507.1227074506192</v>
+      </c>
+      <c r="P71" s="2">
+        <v>185968.03543352999</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>4183.9999999999918</v>
+      </c>
+      <c r="B72" s="2">
+        <v>1005.041577808463</v>
+      </c>
+      <c r="C72" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D72" s="2">
+        <v>2244.722876564279</v>
+      </c>
+      <c r="E72" s="2">
+        <v>97.904702824092013</v>
+      </c>
+      <c r="F72" s="2">
+        <v>83942.996320470527</v>
+      </c>
+      <c r="G72" s="2">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="H72" s="2">
+        <v>15.103657563736149</v>
+      </c>
+      <c r="I72" s="2">
+        <v>2.4573710385786072</v>
+      </c>
+      <c r="J72" s="2">
+        <v>92.937872435693933</v>
+      </c>
+      <c r="K72" s="2">
+        <v>35561.258219050636</v>
+      </c>
+      <c r="L72" s="2">
+        <v>1524.6140846819719</v>
+      </c>
+      <c r="M72" s="2">
+        <v>1134350.952355311</v>
+      </c>
+      <c r="N72" s="2">
+        <v>10.225280638379511</v>
+      </c>
+      <c r="O72" s="2">
+        <v>289.78440425749631</v>
+      </c>
+      <c r="P72" s="2">
+        <v>1130904.8238936481</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>25263.999999999989</v>
+      </c>
+      <c r="B73" s="2">
+        <v>5648.5582401918809</v>
+      </c>
+      <c r="C73" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D73" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E73" s="2">
+        <v>34.266645988432209</v>
+      </c>
+      <c r="F73" s="2">
+        <v>388747.33004037431</v>
+      </c>
+      <c r="G73" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H73" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I73" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J73" s="2">
+        <v>231.3171124750813</v>
+      </c>
+      <c r="K73" s="2">
+        <v>314708.99999999988</v>
+      </c>
+      <c r="L73" s="2">
+        <v>23252.7844053831</v>
+      </c>
+      <c r="M73" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N73" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O73" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P73" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>17569.999999999989</v>
+      </c>
+      <c r="B74" s="2">
+        <v>2404.9664117900902</v>
+      </c>
+      <c r="C74" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D74" s="2">
+        <v>10460.827718341459</v>
+      </c>
+      <c r="E74" s="2">
+        <v>287.5950645457707</v>
+      </c>
+      <c r="F74" s="2">
+        <v>494652.20417661691</v>
+      </c>
+      <c r="G74" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H74" s="2">
+        <v>155.99999999999889</v>
+      </c>
+      <c r="I74" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J74" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K74" s="2">
+        <v>182951.9999999998</v>
+      </c>
+      <c r="L74" s="2">
+        <v>23401.03629808141</v>
+      </c>
+      <c r="M74" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N74" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O74" s="2">
+        <v>909.60104669714224</v>
+      </c>
+      <c r="P74" s="2">
+        <v>486123.80006066471</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>120926</v>
+      </c>
+      <c r="B75" s="2">
+        <v>20038</v>
+      </c>
+      <c r="C75" s="2">
+        <v>29031.0083701363</v>
+      </c>
+      <c r="D75" s="2">
+        <v>72911.599999999991</v>
+      </c>
+      <c r="E75" s="2">
+        <v>2549.9999999999982</v>
+      </c>
+      <c r="F75" s="2">
+        <v>4713511.9352799999</v>
+      </c>
+      <c r="G75" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="H75" s="2">
+        <v>195.99999999999869</v>
+      </c>
+      <c r="I75" s="2">
+        <v>248.99999999999889</v>
+      </c>
+      <c r="J75" s="2">
+        <v>1123.199999999998</v>
+      </c>
+      <c r="K75" s="2">
+        <v>1264806.9999999991</v>
+      </c>
+      <c r="L75" s="2">
+        <v>104307.93</v>
+      </c>
+      <c r="M75" s="2">
+        <v>2214641.3434399972</v>
+      </c>
+      <c r="N75" s="2">
+        <v>34.999999999999908</v>
+      </c>
+      <c r="O75" s="2">
+        <v>6308.9999999999991</v>
+      </c>
+      <c r="P75" s="2">
+        <v>26988496.705479991</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>50473.999999999993</v>
+      </c>
+      <c r="B76" s="2">
+        <v>8680.9999999999982</v>
+      </c>
+      <c r="C76" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D76" s="2">
+        <v>32935.899999999987</v>
+      </c>
+      <c r="E76" s="2">
+        <v>1673.999999999998</v>
+      </c>
+      <c r="F76" s="2">
+        <v>1330729.4930400001</v>
+      </c>
+      <c r="G76" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H76" s="2">
+        <v>158.99999999999889</v>
+      </c>
+      <c r="I76" s="2">
+        <v>184.9999999999992</v>
+      </c>
+      <c r="J76" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K76" s="2">
+        <v>810919.99999999977</v>
+      </c>
+      <c r="L76" s="2">
+        <v>182696</v>
+      </c>
+      <c r="M76" s="2">
+        <v>5519372.8535999991</v>
+      </c>
+      <c r="N76" s="2">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="O76" s="2">
+        <v>2500</v>
+      </c>
+      <c r="P76" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>8854.9999999999945</v>
+      </c>
+      <c r="B77" s="2">
+        <v>1629.211885953139</v>
+      </c>
+      <c r="C77" s="2">
+        <v>2818.518706481017</v>
+      </c>
+      <c r="D77" s="2">
+        <v>347.6177107035295</v>
+      </c>
+      <c r="E77" s="2">
+        <v>415783.74875999981</v>
+      </c>
+      <c r="F77" s="2">
+        <v>67.993988343576362</v>
+      </c>
+      <c r="G77" s="2">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="H77" s="2">
+        <v>19.750936814116528</v>
+      </c>
+      <c r="I77" s="2">
+        <v>19.658968308628911</v>
+      </c>
+      <c r="J77" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K77" s="2">
+        <v>101102.97564972581</v>
+      </c>
+      <c r="L77" s="2">
+        <v>9399.1283429600899</v>
+      </c>
+      <c r="M77" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N77" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O77" s="2">
+        <v>433.52666827411213</v>
+      </c>
+      <c r="P77" s="2">
+        <v>551974.73218514433</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>17833.999999999989</v>
+      </c>
+      <c r="B78" s="2">
+        <v>2658.4559859141509</v>
+      </c>
+      <c r="C78" s="2">
+        <v>7013.1024538403881</v>
+      </c>
+      <c r="D78" s="2">
+        <v>260.09693956895302</v>
+      </c>
+      <c r="E78" s="2">
+        <v>267414.72804000002</v>
+      </c>
+      <c r="F78" s="2">
+        <v>21.713414939660389</v>
+      </c>
+      <c r="G78" s="2">
+        <v>32.08</v>
+      </c>
+      <c r="H78" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I78" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J78" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K78" s="2">
+        <v>297093.99999999983</v>
+      </c>
+      <c r="L78" s="2">
+        <v>20785.402954465699</v>
+      </c>
+      <c r="M78" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N78" s="2">
+        <v>39.999999999999893</v>
+      </c>
+      <c r="O78" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P78" s="2">
+        <v>2364731.1508523719</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>22243.999999999989</v>
+      </c>
+      <c r="B79" s="2">
+        <v>3425.2937930633229</v>
+      </c>
+      <c r="C79" s="2">
+        <v>9827.9147346389273</v>
+      </c>
+      <c r="D79" s="2">
+        <v>252.7008180646225</v>
+      </c>
+      <c r="E79" s="2">
+        <v>229243.99999999991</v>
+      </c>
+      <c r="F79" s="2">
+        <v>14.923705242131829</v>
+      </c>
+      <c r="G79" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H79" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I79" s="2">
+        <v>38.0892510979685</v>
+      </c>
+      <c r="J79" s="2">
+        <v>112.5758503950789</v>
+      </c>
+      <c r="K79" s="2">
+        <v>279415.99999999988</v>
+      </c>
+      <c r="L79" s="2">
+        <v>6034.9460658787029</v>
+      </c>
+      <c r="M79" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N79" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O79" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P79" s="2">
+        <v>907628.90105253621</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>35142.999999999993</v>
+      </c>
+      <c r="B80" s="2">
+        <v>5648.5582401918809</v>
+      </c>
+      <c r="C80" s="2">
+        <v>27639.69999999999</v>
+      </c>
+      <c r="D80" s="2">
+        <v>271.19112182544848</v>
+      </c>
+      <c r="E80" s="2">
+        <v>794230.03655999957</v>
+      </c>
+      <c r="F80" s="2">
+        <v>32.72646118988704</v>
+      </c>
+      <c r="G80" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H80" s="2">
+        <v>125.9999999999992</v>
+      </c>
+      <c r="I80" s="2">
+        <v>95.999999999999559</v>
+      </c>
+      <c r="J80" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K80" s="2">
+        <v>378688.00000000012</v>
+      </c>
+      <c r="L80" s="2">
+        <v>11114.297748609741</v>
+      </c>
+      <c r="M80" s="2">
+        <v>8906174.1647999976</v>
+      </c>
+      <c r="N80" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O80" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P80" s="2">
+        <v>5013077.512856801</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>31885.999999999989</v>
+      </c>
+      <c r="B81" s="2">
+        <v>5652.7282049226433</v>
+      </c>
+      <c r="C81" s="2">
+        <v>10184.16973173145</v>
+      </c>
+      <c r="D81" s="2">
+        <v>424.97873814987389</v>
+      </c>
+      <c r="E81" s="2">
+        <v>135007.86686999991</v>
+      </c>
+      <c r="F81" s="2">
+        <v>6.0474104557206187</v>
+      </c>
+      <c r="G81" s="2">
+        <v>27.965422727272699</v>
+      </c>
+      <c r="H81" s="2">
+        <v>126.9999999999992</v>
+      </c>
+      <c r="I81" s="2">
+        <v>28.665302275848671</v>
+      </c>
+      <c r="J81" s="2">
+        <v>515.09434074171179</v>
+      </c>
+      <c r="K81" s="2">
+        <v>532404</v>
+      </c>
+      <c r="L81" s="2">
+        <v>37819.7689054316</v>
+      </c>
+      <c r="M81" s="2">
+        <v>9174521.0092999972</v>
+      </c>
+      <c r="N81" s="2">
+        <v>29.999999999999918</v>
+      </c>
+      <c r="O81" s="2">
+        <v>2915.7617682164901</v>
+      </c>
+      <c r="P81" s="2">
+        <v>25333054.934995431</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>23671.999999999989</v>
+      </c>
+      <c r="B82" s="2">
+        <v>3592.1638142203678</v>
+      </c>
+      <c r="C82" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D82" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E82" s="2">
+        <v>424.66164849949968</v>
+      </c>
+      <c r="F82" s="2">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G82" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H82" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I82" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J82" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K82" s="2">
+        <v>44036.371116277784</v>
+      </c>
+      <c r="L82" s="2">
+        <v>11411.26707998794</v>
+      </c>
+      <c r="M82" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N82" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O82" s="2">
+        <v>856.70389353902783</v>
+      </c>
+      <c r="P82" s="2">
+        <v>1248365.7581963211</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>116468</v>
+      </c>
+      <c r="B83" s="2">
+        <v>21239</v>
+      </c>
+      <c r="C83" s="2">
+        <v>29031.0083701363</v>
+      </c>
+      <c r="D83" s="2">
+        <v>64664.399999999987</v>
+      </c>
+      <c r="E83" s="2">
+        <v>2077</v>
+      </c>
+      <c r="F83" s="2">
+        <v>4676977.1911800001</v>
+      </c>
+      <c r="G83" s="2">
+        <v>30.2</v>
+      </c>
+      <c r="H83" s="2">
+        <v>300.99999999999812</v>
+      </c>
+      <c r="I83" s="2">
+        <v>303.99999999999869</v>
+      </c>
+      <c r="J83" s="2">
+        <v>783.79999999999882</v>
+      </c>
+      <c r="K83" s="2">
+        <v>202571</v>
+      </c>
+      <c r="L83" s="2">
+        <v>87368.909999999974</v>
+      </c>
+      <c r="M83" s="2">
+        <v>8408723.8795999978</v>
+      </c>
+      <c r="N83" s="2">
+        <v>34.999999999999901</v>
+      </c>
+      <c r="O83" s="2">
+        <v>4502</v>
+      </c>
+      <c r="P83" s="2">
+        <v>25333054.934995431</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>64841.999999999993</v>
+      </c>
+      <c r="B84" s="2">
+        <v>15029</v>
+      </c>
+      <c r="C84" s="2">
+        <v>25869.387780000001</v>
+      </c>
+      <c r="D84" s="2">
+        <v>19151.026043098391</v>
+      </c>
+      <c r="E84" s="2">
+        <v>1645.6410443006489</v>
+      </c>
+      <c r="F84" s="2">
+        <v>1067319.0716998819</v>
+      </c>
+      <c r="G84" s="2">
+        <v>27.620294559099399</v>
+      </c>
+      <c r="H84" s="2">
+        <v>124.9999999999992</v>
+      </c>
+      <c r="I84" s="2">
+        <v>194.99999999999909</v>
+      </c>
+      <c r="J84" s="2">
+        <v>384.78892776104192</v>
+      </c>
+      <c r="K84" s="2">
+        <v>2168.999999999995</v>
+      </c>
+      <c r="L84" s="2">
+        <v>24766.251315762191</v>
+      </c>
+      <c r="M84" s="2">
+        <v>282905.75142886041</v>
+      </c>
+      <c r="N84" s="2">
+        <v>21.095615783084529</v>
+      </c>
+      <c r="O84" s="2">
+        <v>3211</v>
+      </c>
+      <c r="P84" s="2">
+        <v>9430951.7147999946</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>64100</v>
+      </c>
+      <c r="B85" s="2">
+        <v>9192</v>
+      </c>
+      <c r="C85" s="2">
+        <v>21205.026720000002</v>
+      </c>
+      <c r="D85" s="2">
+        <v>59994</v>
+      </c>
+      <c r="E85" s="2">
+        <v>1042.9999999999991</v>
+      </c>
+      <c r="F85" s="2">
+        <v>1194600.348719999</v>
+      </c>
+      <c r="G85" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H85" s="2">
+        <v>140.99999999999909</v>
+      </c>
+      <c r="I85" s="2">
+        <v>92.999999999999559</v>
+      </c>
+      <c r="J85" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K85" s="2">
+        <v>39877.133642530513</v>
+      </c>
+      <c r="L85" s="2">
+        <v>70633.640917482451</v>
+      </c>
+      <c r="M85" s="2">
+        <v>8271274.1760000018</v>
+      </c>
+      <c r="N85" s="2">
+        <v>36.999999999999908</v>
+      </c>
+      <c r="O85" s="2">
+        <v>3090</v>
+      </c>
+      <c r="P85" s="2">
+        <v>7029925.2345599988</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>105038</v>
+      </c>
+      <c r="B86" s="2">
+        <v>11442</v>
+      </c>
+      <c r="C86" s="2">
         <v>24430.417592114401</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D86" s="2">
         <v>69421.599999999991</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E86" s="2">
         <v>96.75042719463211</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F86" s="2">
         <v>3389505.0556999999</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G86" s="2">
         <v>27.620294559099399</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H86" s="2">
         <v>164.99999999999889</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I86" s="2">
         <v>248.99999999999901</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J86" s="2">
         <v>384.78892776104192</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K86" s="2">
         <v>28977.998578687861</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L86" s="2">
         <v>57789.999999999949</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M86" s="2">
         <v>827690.06333850382</v>
       </c>
-      <c r="N46" s="2">
+      <c r="N86" s="2">
         <v>5.9999999999999627</v>
       </c>
-      <c r="O46" s="2">
+      <c r="O86" s="2">
         <v>3403</v>
       </c>
-      <c r="P46" s="2">
+      <c r="P86" s="2">
         <v>8379778.1909793671</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>22677.999999999989</v>
+      </c>
+      <c r="B87" s="2">
+        <v>3245.6856023523028</v>
+      </c>
+      <c r="C87" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D87" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E87" s="2">
+        <v>881.00766886934832</v>
+      </c>
+      <c r="F87" s="2">
+        <v>653758.65263628191</v>
+      </c>
+      <c r="G87" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H87" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I87" s="2">
+        <v>40.546622136547143</v>
+      </c>
+      <c r="J87" s="2">
+        <v>303.47526404677512</v>
+      </c>
+      <c r="K87" s="2">
+        <v>16059.27802363551</v>
+      </c>
+      <c r="L87" s="2">
+        <v>43983.130421927461</v>
+      </c>
+      <c r="M87" s="2">
+        <v>1887136.8709383111</v>
+      </c>
+      <c r="N87" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O87" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P87" s="2">
+        <v>1405933.835730277</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>17174.999999999989</v>
+      </c>
+      <c r="B88" s="2">
+        <v>2969.2673230310902</v>
+      </c>
+      <c r="C88" s="2">
+        <v>22823.19152</v>
+      </c>
+      <c r="D88" s="2">
+        <v>8278.1089937218167</v>
+      </c>
+      <c r="E88" s="2">
+        <v>299.83315239878198</v>
+      </c>
+      <c r="F88" s="2">
+        <v>341503.88560920162</v>
+      </c>
+      <c r="G88" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H88" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I88" s="2">
+        <v>9.8294841543144464</v>
+      </c>
+      <c r="J88" s="2">
+        <v>92.823698145232413</v>
+      </c>
+      <c r="K88" s="2">
+        <v>101102.97564972581</v>
+      </c>
+      <c r="L88" s="2">
+        <v>19534.248129094489</v>
+      </c>
+      <c r="M88" s="2">
+        <v>2462949.6162042459</v>
+      </c>
+      <c r="N88" s="2">
+        <v>16.360449021407241</v>
+      </c>
+      <c r="O88" s="2">
+        <v>839.45482185703395</v>
+      </c>
+      <c r="P88" s="2">
+        <v>2202359.3255764418</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>39066.999999999993</v>
+      </c>
+      <c r="B89" s="2">
+        <v>6011.9999999999982</v>
+      </c>
+      <c r="C89" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D89" s="2">
+        <v>20455.999999999989</v>
+      </c>
+      <c r="E89" s="2">
+        <v>881.00766886934832</v>
+      </c>
+      <c r="F89" s="2">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G89" s="2">
+        <v>37.19</v>
+      </c>
+      <c r="H89" s="2">
+        <v>147.99999999999909</v>
+      </c>
+      <c r="I89" s="2">
+        <v>77.805859831260051</v>
+      </c>
+      <c r="J89" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K89" s="2">
+        <v>30021.162791278759</v>
+      </c>
+      <c r="L89" s="2">
+        <v>32411.801282762281</v>
+      </c>
+      <c r="M89" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N89" s="2">
+        <v>35.752251160859089</v>
+      </c>
+      <c r="O89" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P89" s="2">
+        <v>6067714.9468499981</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>27626.999999999989</v>
+      </c>
+      <c r="B90" s="2">
+        <v>5648.5582401918809</v>
+      </c>
+      <c r="C90" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D90" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E90" s="2">
+        <v>1097.9999999999991</v>
+      </c>
+      <c r="F90" s="2">
+        <v>1094086.860592877</v>
+      </c>
+      <c r="G90" s="2">
+        <v>51.2</v>
+      </c>
+      <c r="H90" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I90" s="2">
+        <v>45.461364213704371</v>
+      </c>
+      <c r="J90" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K90" s="2">
+        <v>43145.423345459072</v>
+      </c>
+      <c r="L90" s="2">
+        <v>32808.740488069772</v>
+      </c>
+      <c r="M90" s="2">
+        <v>4717355.206267274</v>
+      </c>
+      <c r="N90" s="2">
+        <v>17.382977085245191</v>
+      </c>
+      <c r="O90" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P90" s="2">
+        <v>838720.66501022666</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>31271</v>
+      </c>
+      <c r="B91" s="2">
+        <v>5648.5582401918809</v>
+      </c>
+      <c r="C91" s="2">
+        <v>20815.4167831292</v>
+      </c>
+      <c r="D91" s="2">
+        <v>19721.961700869851</v>
+      </c>
+      <c r="E91" s="2">
+        <v>881.00766886934832</v>
+      </c>
+      <c r="F91" s="2">
+        <v>452394.49636074452</v>
+      </c>
+      <c r="G91" s="2">
+        <v>30.831632653061199</v>
+      </c>
+      <c r="H91" s="2">
+        <v>125.6772308691166</v>
+      </c>
+      <c r="I91" s="2">
+        <v>113.9999999999995</v>
+      </c>
+      <c r="J91" s="2">
+        <v>657.77532591485419</v>
+      </c>
+      <c r="K91" s="2">
+        <v>116218</v>
+      </c>
+      <c r="L91" s="2">
+        <v>36514.425245026046</v>
+      </c>
+      <c r="M91" s="2">
+        <v>5228156.3358999994</v>
+      </c>
+      <c r="N91" s="2">
+        <v>38.999999999999908</v>
+      </c>
+      <c r="O91" s="2">
+        <v>1599.139320430128</v>
+      </c>
+      <c r="P91" s="2">
+        <v>5013077.512856801</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>